<commit_message>
implemented low hp visual
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrie\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DD6EE6-BFDA-4525-8B4E-FF8382BD6019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F60DF0-1776-4AC8-AB32-B491202609E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -148,10 +148,25 @@
     <t>(Plusieurs éléments)</t>
   </si>
   <si>
-    <t>Not started</t>
+    <t>Implement new sprite sheet (polish)</t>
   </si>
   <si>
-    <t/>
+    <t>Correct small bugs</t>
+  </si>
+  <si>
+    <t>Improve global structure</t>
+  </si>
+  <si>
+    <t>Player instantiation will now be automatic + aura is correctly disabled on main menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Total hours spend on project</t>
+  </si>
+  <si>
+    <t>Is passive</t>
   </si>
 </sst>
 </file>
@@ -162,10 +177,10 @@
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    <numFmt numFmtId="167" formatCode="h&quot;h&quot;mm;@"/>
     <numFmt numFmtId="168" formatCode="d/m/yy\ hh:mm;@"/>
+    <numFmt numFmtId="171" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +208,22 @@
       <name val="Avenir Next LT Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,7 +233,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -262,11 +293,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -294,18 +343,259 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="171" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -338,19 +628,10 @@
       <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="h&quot;h&quot;mm;@"/>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
     </dxf>
     <dxf>
       <font>
@@ -445,35 +726,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
     </dxf>
     <dxf>
       <font>
@@ -909,16 +1161,16 @@
                 <c:formatCode>h"h"\ mm"min";@</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.1423611111111111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14374999999999999</c:v>
+                  <c:v>0.16944444444444445</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4722222222222224E-2</c:v>
+                  <c:v>7.013888888888889E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1735,21 +1987,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45288.433955902779" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45288.722229976855" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tasks"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Feature/Task" numFmtId="0">
-      <sharedItems containsBlank="1" count="7">
-        <s v="Create TimeManagement system"/>
-        <s v="Play Test"/>
-        <s v="TimeManagment maintenance"/>
-        <s v="Make low HP visuals"/>
-        <s v="Implement low HP visuals"/>
-        <s v="Make falling sprite + polish sprite sheet"/>
-        <m/>
-      </sharedItems>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Desciption" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -1764,22 +2008,20 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Started" numFmtId="168">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2023-12-28T09:16:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2023-12-28T16:06:00"/>
     </cacheField>
     <cacheField name="Ended" numFmtId="168">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2023-12-27T20:03:00" count="2">
-        <d v="2023-12-27T20:03:00"/>
-        <m/>
-      </sharedItems>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2023-12-28T16:06:00"/>
     </cacheField>
     <cacheField name="Total time" numFmtId="165">
       <sharedItems containsDate="1" containsMixedTypes="1" minDate="1899-12-30T00:25:00" maxDate="1899-12-30T03:02:00"/>
     </cacheField>
     <cacheField name="Finished" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
+      <sharedItems containsBlank="1" count="4">
         <b v="1"/>
         <b v="0"/>
-        <m/>
+        <s v=""/>
+        <m u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1794,443 +2036,443 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="49">
   <r>
-    <x v="0"/>
+    <s v="Create TimeManagement system"/>
     <s v="Manage time more efficiently by tracking tasks and time taken"/>
     <x v="0"/>
     <d v="2023-12-27T15:25:00"/>
-    <x v="0"/>
+    <d v="2023-12-27T20:03:00"/>
     <d v="1899-12-30T03:02:00"/>
     <x v="0"/>
   </r>
   <r>
-    <x v="1"/>
+    <s v="Play Test"/>
     <s v="Play test the game to collect feedback"/>
     <x v="1"/>
     <d v="2023-12-27T16:45:00"/>
-    <x v="1"/>
+    <m/>
     <d v="1899-12-30T00:30:00"/>
     <x v="1"/>
   </r>
   <r>
-    <x v="2"/>
+    <s v="TimeManagment maintenance"/>
     <s v="Tweak and update small things for better management"/>
     <x v="0"/>
     <d v="2023-12-28T08:13:00"/>
+    <m/>
+    <d v="1899-12-30T01:02:00"/>
     <x v="1"/>
+  </r>
+  <r>
+    <s v="Make low HP visuals"/>
+    <m/>
+    <x v="2"/>
+    <d v="2023-12-28T08:57:00"/>
+    <m/>
     <d v="1899-12-30T00:25:00"/>
     <x v="1"/>
   </r>
   <r>
+    <s v="Implement low HP visuals"/>
+    <m/>
     <x v="3"/>
-    <m/>
-    <x v="2"/>
-    <d v="2023-12-28T08:57:00"/>
-    <x v="1"/>
-    <d v="1899-12-30T00:25:00"/>
-    <x v="1"/>
+    <d v="2023-12-28T09:00:00"/>
+    <d v="2023-12-28T16:06:00"/>
+    <d v="1899-12-30T02:38:00"/>
+    <x v="0"/>
   </r>
   <r>
-    <x v="4"/>
+    <s v="Make falling sprite + polish sprite sheet"/>
+    <m/>
+    <x v="2"/>
+    <d v="2023-12-28T09:16:00"/>
+    <d v="2023-12-28T11:24:00"/>
+    <d v="1899-12-30T01:16:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Implement new sprite sheet (polish)"/>
     <m/>
     <x v="3"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v="Not started"/>
     <x v="1"/>
   </r>
   <r>
-    <x v="5"/>
-    <m/>
-    <x v="2"/>
-    <d v="2023-12-28T09:16:00"/>
-    <x v="1"/>
-    <d v="1899-12-30T00:25:00"/>
+    <s v="Improve global structure"/>
+    <m/>
+    <x v="3"/>
+    <d v="2023-12-28T16:06:00"/>
+    <m/>
+    <d v="1899-12-30T00:47:00"/>
     <x v="1"/>
   </r>
   <r>
-    <x v="6"/>
+    <s v="Correct small bugs"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <m/>
+    <s v="Not started"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <m/>
     <m/>
     <x v="4"/>
     <m/>
-    <x v="1"/>
-    <s v=""/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <m/>
-    <x v="4"/>
-    <m/>
-    <x v="1"/>
-    <s v=""/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <m/>
-    <x v="4"/>
-    <m/>
-    <x v="1"/>
-    <s v=""/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <m/>
-    <x v="4"/>
-    <m/>
-    <x v="1"/>
+    <m/>
     <s v=""/>
     <x v="2"/>
   </r>
@@ -2238,21 +2480,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="6">
@@ -2265,18 +2496,13 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
+      <items count="5">
         <item x="1"/>
         <item x="0"/>
+        <item h="1" m="1" x="3"/>
         <item h="1" x="2"/>
         <item t="default"/>
       </items>
@@ -2312,7 +2538,7 @@
     <dataField name="Somme de Total time" fld="5" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="4">
+    <format dxfId="30">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2340,31 +2566,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:G50" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:G50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:H50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="3">
+      <calculatedColumnFormula>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="1">
+      <calculatedColumnFormula>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:E50" xr:uid="{341A430F-6539-4177-979B-C2093504802E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="5">
-      <calculatedColumnFormula>IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="0">
+      <calculatedColumnFormula>IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2635,25 +2870,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:K108"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="75.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="5" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="74.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2675,16 +2913,19 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2694,29 +2935,36 @@
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>45287.642361111109</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>45287.835416666669</v>
       </c>
-      <c r="F2" s="4" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="G2" s="2" t="b">
-        <v>1</v>
+      <c r="F2" s="4">
+        <f ca="1">_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v>0.12638888888614019</v>
+      </c>
+      <c r="G2" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v>YES</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="8" t="b">
+      <c r="K2" s="2"/>
+      <c r="L2" s="8" t="b">
         <f>1=1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2726,27 +2974,36 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <v>45287.697916666664</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="4" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="9" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="4">
+        <f ca="1">_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v>2.0833333335758653E-2</v>
+      </c>
+      <c r="G3" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v>NO</v>
+      </c>
+      <c r="H3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="10" t="b">
+      <c r="K3" s="2"/>
+      <c r="L3" s="10" t="b">
         <f>1=0</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2756,24 +3013,33 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>45288.342361111114</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="4" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="G4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="9" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="4">
+        <f ca="1">_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v>4.3055555550381541E-2</v>
+      </c>
+      <c r="G4" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v>NO</v>
+      </c>
+      <c r="H4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -2781,24 +3047,33 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>45288.372916666667</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="4" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="G5" s="2" t="b">
-        <v>0</v>
+      <c r="E5" s="13">
+        <v>45288.395833333336</v>
+      </c>
+      <c r="F5" s="4">
+        <f ca="1">_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v>1.7361111116770189E-2</v>
+      </c>
+      <c r="G5" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v>YES</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -2806,22 +3081,33 @@
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="2" t="b">
-        <v>0</v>
+      <c r="D6" s="13">
+        <v>45288.375</v>
+      </c>
+      <c r="E6" s="13">
+        <v>45288.67083333333</v>
+      </c>
+      <c r="F6" s="4">
+        <f ca="1">_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v>0.10972222221607808</v>
+      </c>
+      <c r="G6" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v>YES</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="2"/>
+      <c r="J6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -2829,669 +3115,1079 @@
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>45288.386111111111</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="4" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="G7" s="2" t="b">
-        <v>0</v>
+      <c r="E7" s="13">
+        <v>45288.474999999999</v>
+      </c>
+      <c r="F7" s="4">
+        <f ca="1">_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v>5.2777777775190771E-2</v>
+      </c>
+      <c r="G7" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v>YES</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="2"/>
+      <c r="J7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v>Not started</v>
+      </c>
+      <c r="G8" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v>NO</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="13">
+        <v>45288.67083333333</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="4">
+        <f ca="1">_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v>3.680555555911269E-2</v>
+      </c>
+      <c r="G9" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v>NO</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v>Not started</v>
+      </c>
+      <c r="G10" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v>NO</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="2"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G11" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="2"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G12" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="2"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G13" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="2"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G14" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="2"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G15" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="2"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G16" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="2"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G17" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="2"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G18" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="2"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G19" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="2"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G20" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="2"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G21" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="2"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G22" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="2"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G23" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="2"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G24" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="2"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G25" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="2"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G26" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="2"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G27" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" s="2"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G28" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G29" s="2"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G29" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="2"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G30" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G31" s="2"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G31" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G32" s="2"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G32" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G33" s="2"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G33" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" s="2"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G34" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" s="2"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G35" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G36" s="2"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G36" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G37" s="2"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G37" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G38" s="2"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G38" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G39" s="2"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G39" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G40" s="2"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G40" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G41" s="2"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G41" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G42" s="2"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G42" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G43" s="2"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G43" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G44" s="2"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G44" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G45" s="2"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G45" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G46" s="2"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G46" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G47" s="2"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G47" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G48" s="2"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G48" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G49" s="2"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G49" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G50" s="2"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="4" t="str">
+        <f>_xlfn.LET(
+_xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
+_xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
+IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
+)</f>
+        <v/>
+      </c>
+      <c r="G50" s="23" t="str">
+        <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
+        <v/>
+      </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3499,8 +4195,9 @@
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -3508,8 +4205,9 @@
       <c r="E60" s="3"/>
       <c r="F60" s="4"/>
       <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -3517,8 +4215,9 @@
       <c r="E61" s="3"/>
       <c r="F61" s="4"/>
       <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -3526,8 +4225,9 @@
       <c r="E62" s="3"/>
       <c r="F62" s="4"/>
       <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -3535,8 +4235,9 @@
       <c r="E63" s="3"/>
       <c r="F63" s="4"/>
       <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3544,8 +4245,9 @@
       <c r="E64" s="3"/>
       <c r="F64" s="4"/>
       <c r="G64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -3553,8 +4255,9 @@
       <c r="E65" s="3"/>
       <c r="F65" s="4"/>
       <c r="G65" s="2"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -3562,8 +4265,9 @@
       <c r="E66" s="3"/>
       <c r="F66" s="4"/>
       <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -3571,8 +4275,9 @@
       <c r="E67" s="3"/>
       <c r="F67" s="4"/>
       <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3580,8 +4285,9 @@
       <c r="E68" s="3"/>
       <c r="F68" s="4"/>
       <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -3589,8 +4295,9 @@
       <c r="E69" s="3"/>
       <c r="F69" s="4"/>
       <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -3598,8 +4305,9 @@
       <c r="E70" s="3"/>
       <c r="F70" s="4"/>
       <c r="G70" s="2"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -3607,8 +4315,9 @@
       <c r="E71" s="3"/>
       <c r="F71" s="4"/>
       <c r="G71" s="2"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -3616,8 +4325,9 @@
       <c r="E72" s="3"/>
       <c r="F72" s="4"/>
       <c r="G72" s="2"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3625,8 +4335,9 @@
       <c r="E73" s="3"/>
       <c r="F73" s="4"/>
       <c r="G73" s="2"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3634,8 +4345,9 @@
       <c r="E74" s="3"/>
       <c r="F74" s="4"/>
       <c r="G74" s="2"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3643,8 +4355,9 @@
       <c r="E75" s="3"/>
       <c r="F75" s="4"/>
       <c r="G75" s="2"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3652,8 +4365,9 @@
       <c r="E76" s="3"/>
       <c r="F76" s="4"/>
       <c r="G76" s="2"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3661,8 +4375,9 @@
       <c r="E77" s="3"/>
       <c r="F77" s="4"/>
       <c r="G77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3670,8 +4385,9 @@
       <c r="E78" s="3"/>
       <c r="F78" s="4"/>
       <c r="G78" s="2"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3679,8 +4395,9 @@
       <c r="E79" s="3"/>
       <c r="F79" s="4"/>
       <c r="G79" s="2"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -3688,8 +4405,9 @@
       <c r="E80" s="3"/>
       <c r="F80" s="4"/>
       <c r="G80" s="2"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -3697,8 +4415,9 @@
       <c r="E81" s="3"/>
       <c r="F81" s="4"/>
       <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3706,8 +4425,9 @@
       <c r="E82" s="3"/>
       <c r="F82" s="4"/>
       <c r="G82" s="2"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="2"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3715,8 +4435,9 @@
       <c r="E83" s="3"/>
       <c r="F83" s="4"/>
       <c r="G83" s="2"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="2"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3724,8 +4445,9 @@
       <c r="E84" s="3"/>
       <c r="F84" s="4"/>
       <c r="G84" s="2"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="2"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3733,8 +4455,9 @@
       <c r="E85" s="3"/>
       <c r="F85" s="4"/>
       <c r="G85" s="2"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3742,8 +4465,9 @@
       <c r="E86" s="3"/>
       <c r="F86" s="4"/>
       <c r="G86" s="2"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86" s="2"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -3751,8 +4475,9 @@
       <c r="E87" s="3"/>
       <c r="F87" s="4"/>
       <c r="G87" s="2"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87" s="2"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -3760,8 +4485,9 @@
       <c r="E88" s="3"/>
       <c r="F88" s="4"/>
       <c r="G88" s="2"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3769,8 +4495,9 @@
       <c r="E89" s="3"/>
       <c r="F89" s="4"/>
       <c r="G89" s="2"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="2"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3778,8 +4505,9 @@
       <c r="E90" s="3"/>
       <c r="F90" s="4"/>
       <c r="G90" s="2"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="2"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3787,8 +4515,9 @@
       <c r="E91" s="3"/>
       <c r="F91" s="4"/>
       <c r="G91" s="2"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="2"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3796,8 +4525,9 @@
       <c r="E92" s="3"/>
       <c r="F92" s="4"/>
       <c r="G92" s="2"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="2"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3805,8 +4535,9 @@
       <c r="E93" s="3"/>
       <c r="F93" s="4"/>
       <c r="G93" s="2"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="2"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3814,8 +4545,9 @@
       <c r="E94" s="3"/>
       <c r="F94" s="4"/>
       <c r="G94" s="2"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="2"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3823,8 +4555,9 @@
       <c r="E95" s="3"/>
       <c r="F95" s="4"/>
       <c r="G95" s="2"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="2"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3832,8 +4565,9 @@
       <c r="E96" s="3"/>
       <c r="F96" s="4"/>
       <c r="G96" s="2"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96" s="2"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3841,8 +4575,9 @@
       <c r="E97" s="3"/>
       <c r="F97" s="4"/>
       <c r="G97" s="2"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="2"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3850,8 +4585,9 @@
       <c r="E98" s="3"/>
       <c r="F98" s="4"/>
       <c r="G98" s="2"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="2"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3859,8 +4595,9 @@
       <c r="E99" s="3"/>
       <c r="F99" s="4"/>
       <c r="G99" s="2"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="2"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3868,8 +4605,9 @@
       <c r="E100" s="3"/>
       <c r="F100" s="4"/>
       <c r="G100" s="2"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="2"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3877,8 +4615,9 @@
       <c r="E101" s="3"/>
       <c r="F101" s="4"/>
       <c r="G101" s="2"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101" s="2"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3886,8 +4625,9 @@
       <c r="E102" s="3"/>
       <c r="F102" s="4"/>
       <c r="G102" s="2"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="2"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3895,8 +4635,9 @@
       <c r="E103" s="3"/>
       <c r="F103" s="4"/>
       <c r="G103" s="2"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H103" s="2"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3904,8 +4645,9 @@
       <c r="E104" s="3"/>
       <c r="F104" s="4"/>
       <c r="G104" s="2"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104" s="2"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3913,8 +4655,9 @@
       <c r="E105" s="3"/>
       <c r="F105" s="4"/>
       <c r="G105" s="2"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H105" s="2"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3922,8 +4665,9 @@
       <c r="E106" s="3"/>
       <c r="F106" s="4"/>
       <c r="G106" s="2"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="2"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3931,8 +4675,9 @@
       <c r="E107" s="3"/>
       <c r="F107" s="4"/>
       <c r="G107" s="2"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107" s="2"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3940,30 +4685,34 @@
       <c r="E108" s="3"/>
       <c r="F108" s="4"/>
       <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G50">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>AND(NOT($G2), $A2 &lt;&gt; "")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$G2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G60:G108">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="G60:H108">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>AND(NOT($G60), $A60 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>$G60</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G50">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$G2="YES"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>AND(NOT($G2 = "YES"), $A2 &lt;&gt; "")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$H2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G50 G60:G108" xr:uid="{205D516F-C074-4903-A0E9-4E3F9518DD6F}">
-      <formula1>$K$2:$K$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50 C60:C108" xr:uid="{DC5BF156-2602-425B-86A0-7257C6F2DA5F}">
+      <formula1>$J$2:$J$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50 C60:C108" xr:uid="{DC5BF156-2602-425B-86A0-7257C6F2DA5F}">
-      <formula1>$I$2:$I$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H50" xr:uid="{D6219296-ED51-4D3C-BCB2-1138D9D7567E}">
+      <formula1>$L$2:$L$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3976,21 +4725,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1250E3B8-C8C4-41E1-8291-CCD286903BDF}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" customWidth="1"/>
     <col min="3" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -4007,7 +4756,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -4018,12 +4767,12 @@
       <c r="D2" s="12">
         <v>45287.834722222222</v>
       </c>
-      <c r="E2" s="13">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E2" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>0.12638888888614019</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -4036,12 +4785,12 @@
       <c r="D3" s="12">
         <v>45287.708333333336</v>
       </c>
-      <c r="E3" s="13">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E3" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.0416666671517305E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -4052,12 +4801,12 @@
       <c r="D4" s="12">
         <v>45288.361805555556</v>
       </c>
-      <c r="E4" s="13">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E4" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.7361111109494232E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -4070,12 +4819,12 @@
       <c r="D5" s="12">
         <v>45288.372916666667</v>
       </c>
-      <c r="E5" s="13">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E5" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.0416666664241347E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -4086,12 +4835,12 @@
       <c r="D6" s="12">
         <v>45288.395833333336</v>
       </c>
-      <c r="E6" s="13">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E6" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.7361111116770189E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -4102,12 +4851,19 @@
       <c r="D7" s="12">
         <v>45288.413194444445</v>
       </c>
-      <c r="E7" s="13">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E7" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.7361111109494232E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -4118,12 +4874,17 @@
       <c r="D8" s="12">
         <v>45288.439583333333</v>
       </c>
-      <c r="E8" s="13">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E8" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>2.569444444088731E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -4134,12 +4895,20 @@
       <c r="D9" s="12">
         <v>45288.474999999999</v>
       </c>
-      <c r="E9" s="13">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E9" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>3.5416666665696539E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="20">
+        <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
+        <v>0.40694444443943212</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -4150,68 +4919,100 @@
       <c r="D10" s="12">
         <v>45288.488888888889</v>
       </c>
-      <c r="E10" s="13">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E10" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.1111111110949423E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="C11" s="12">
+        <v>45288.531944444447</v>
+      </c>
+      <c r="D11" s="12">
+        <v>45288.540277777778</v>
+      </c>
+      <c r="E11" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
+        <v>8.333333331393078E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="C12" s="12">
+        <v>45288.580555555556</v>
+      </c>
+      <c r="D12" s="12">
+        <v>45288.67083333333</v>
+      </c>
+      <c r="E12" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
+        <v>9.0277777773735579E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="12">
+        <v>45288.671527777777</v>
+      </c>
+      <c r="D13" s="12">
+        <v>45288.70416666667</v>
+      </c>
+      <c r="E13" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
+        <v>3.2638888893416151E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="12">
+        <v>45288.734027777777</v>
+      </c>
+      <c r="D14" s="12">
+        <v>45288.738194444442</v>
+      </c>
+      <c r="E14" s="17">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
+        <v>4.166666665696539E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
+        <v/>
+      </c>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E16" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4220,8 +5021,8 @@
       <c r="B17" s="2"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E17" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4230,8 +5031,8 @@
       <c r="B18" s="2"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E18" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4240,8 +5041,8 @@
       <c r="B19" s="2"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E19" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4250,8 +5051,8 @@
       <c r="B20" s="2"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E20" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4260,8 +5061,8 @@
       <c r="B21" s="2"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E21" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4270,8 +5071,8 @@
       <c r="B22" s="2"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
-      <c r="E22" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E22" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4280,8 +5081,8 @@
       <c r="B23" s="2"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E23" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4290,8 +5091,8 @@
       <c r="B24" s="2"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
-      <c r="E24" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E24" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4300,8 +5101,8 @@
       <c r="B25" s="2"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
-      <c r="E25" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E25" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4310,8 +5111,8 @@
       <c r="B26" s="2"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E26" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4320,8 +5121,8 @@
       <c r="B27" s="2"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E27" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4330,8 +5131,8 @@
       <c r="B28" s="2"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E28" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4340,8 +5141,8 @@
       <c r="B29" s="2"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
-      <c r="E29" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E29" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4350,8 +5151,8 @@
       <c r="B30" s="2"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E30" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4360,8 +5161,8 @@
       <c r="B31" s="2"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E31" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4370,8 +5171,8 @@
       <c r="B32" s="2"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
-      <c r="E32" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E32" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4380,8 +5181,8 @@
       <c r="B33" s="2"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
-      <c r="E33" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E33" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4390,8 +5191,8 @@
       <c r="B34" s="2"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
-      <c r="E34" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E34" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4400,8 +5201,8 @@
       <c r="B35" s="2"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
-      <c r="E35" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E35" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4410,8 +5211,8 @@
       <c r="B36" s="2"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
-      <c r="E36" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E36" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4420,8 +5221,8 @@
       <c r="B37" s="2"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
-      <c r="E37" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E37" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4430,8 +5231,8 @@
       <c r="B38" s="2"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
-      <c r="E38" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E38" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4440,8 +5241,8 @@
       <c r="B39" s="2"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
-      <c r="E39" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E39" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4450,8 +5251,8 @@
       <c r="B40" s="2"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
-      <c r="E40" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E40" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4460,8 +5261,8 @@
       <c r="B41" s="2"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
-      <c r="E41" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E41" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4470,8 +5271,8 @@
       <c r="B42" s="2"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
-      <c r="E42" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E42" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4480,8 +5281,8 @@
       <c r="B43" s="2"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
-      <c r="E43" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E43" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4490,8 +5291,8 @@
       <c r="B44" s="2"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
-      <c r="E44" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E44" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4500,8 +5301,8 @@
       <c r="B45" s="2"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
-      <c r="E45" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E45" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4510,8 +5311,8 @@
       <c r="B46" s="2"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
-      <c r="E46" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E46" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4520,8 +5321,8 @@
       <c r="B47" s="2"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
-      <c r="E47" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E47" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4530,8 +5331,8 @@
       <c r="B48" s="2"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
-      <c r="E48" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E48" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4540,8 +5341,8 @@
       <c r="B49" s="2"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
-      <c r="E49" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E49" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -4550,12 +5351,16 @@
       <c r="B50" s="2"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
-      <c r="E50" s="13" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],"Current session : " &amp; TEXT(NOW()-Sessions[[#This Row],[Session start]],"h""h""mm""m""ss""s""")), "")</f>
+      <c r="E50" s="17" t="str">
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F7:J8"/>
+    <mergeCell ref="F9:J10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -4577,10 +5382,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F34BC3-EAE3-4982-A7A6-05997E0322BF}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4596,7 +5401,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
@@ -4604,7 +5409,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B3" t="s">
@@ -4612,43 +5417,48 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="17">
-        <v>0</v>
+      <c r="B4" s="16">
+        <v>0.1423611111111111</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="17">
-        <v>0.14374999999999999</v>
+      <c r="B5" s="16">
+        <v>0.16944444444444445</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="17">
-        <v>3.4722222222222224E-2</v>
+      <c r="B7" s="16">
+        <v>7.013888888888889E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="17">
-        <v>0.19930555555555557</v>
+      <c r="B8" s="16">
+        <v>0.40277777777777779</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made better level 1 and added some animation scripts
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrie\Desktop\Projects\Unity\Project - Find Mocha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F60DF0-1776-4AC8-AB32-B491202609E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51933E3A-3DDB-4528-8FCF-1590BCEC2C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="12" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -168,6 +168,15 @@
   <si>
     <t>Is passive</t>
   </si>
+  <si>
+    <t>Create new levels (level design)</t>
+  </si>
+  <si>
+    <t>Level design</t>
+  </si>
+  <si>
+    <t>Correct tilemap collider</t>
+  </si>
 </sst>
 </file>
 
@@ -177,10 +186,10 @@
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    <numFmt numFmtId="168" formatCode="d/m/yy\ hh:mm;@"/>
-    <numFmt numFmtId="171" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
+    <numFmt numFmtId="167" formatCode="d/m/yy\ hh:mm;@"/>
+    <numFmt numFmtId="168" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +232,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Avenir Next LT Pro"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -343,22 +359,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -367,39 +384,76 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="26">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="171" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <color theme="2" tint="-0.499984740745262"/>
         <name val="Avenir Next LT Pro"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -437,201 +491,19 @@
       <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
-        <b val="0"/>
-        <i/>
-        <color theme="6" tint="-0.24994659260841701"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+      <numFmt numFmtId="168" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
     </dxf>
     <dxf>
       <font>
@@ -740,7 +612,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="168" formatCode="d/m/yy\ hh:mm;@"/>
+      <numFmt numFmtId="167" formatCode="d/m/yy\ hh:mm;@"/>
     </dxf>
     <dxf>
       <font>
@@ -755,7 +627,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="168" formatCode="d/m/yy\ hh:mm;@"/>
+      <numFmt numFmtId="167" formatCode="d/m/yy\ hh:mm;@"/>
     </dxf>
     <dxf>
       <font>
@@ -1136,9 +1008,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Charts!$A$4:$A$8</c:f>
+              <c:f>Charts!$A$4:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Coding</c:v>
                 </c:pt>
@@ -1151,17 +1023,20 @@
                 <c:pt idx="3">
                   <c:v>Sprite assets</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>Level design</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$B$4:$B$8</c:f>
+              <c:f>Charts!$B$4:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>h"h"\ mm"min";@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.1423611111111111</c:v>
+                  <c:v>0.23611111111111113</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.16944444444444445</c:v>
@@ -1171,6 +1046,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.013888888888889E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1987,11 +1865,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45288.722229976855" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45292.949456365743" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tasks"/>
   </cacheSource>
-  <cacheFields count="7">
+  <cacheFields count="8">
     <cacheField name="Feature/Task" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
@@ -1999,30 +1877,36 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Task Type" numFmtId="0">
-      <sharedItems containsBlank="1" count="5">
+      <sharedItems containsBlank="1" count="6">
         <s v="Management"/>
         <s v="Playtesting"/>
         <s v="Sprite assets"/>
         <s v="Coding"/>
+        <s v="Level design"/>
         <m/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Started" numFmtId="168">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2023-12-28T16:06:00"/>
+    <cacheField name="Started" numFmtId="167">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2024-01-01T20:00:00"/>
     </cacheField>
-    <cacheField name="Ended" numFmtId="168">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2023-12-28T16:06:00"/>
+    <cacheField name="Ended" numFmtId="167">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2024-01-01T22:41:00"/>
     </cacheField>
     <cacheField name="Total time" numFmtId="165">
       <sharedItems containsDate="1" containsMixedTypes="1" minDate="1899-12-30T00:25:00" maxDate="1899-12-30T03:02:00"/>
     </cacheField>
     <cacheField name="Finished" numFmtId="0">
-      <sharedItems containsBlank="1" count="4">
-        <b v="1"/>
-        <b v="0"/>
+      <sharedItems containsBlank="1" count="6">
+        <s v="YES"/>
+        <s v="NO"/>
         <s v=""/>
+        <b v="1" u="1"/>
+        <b v="0" u="1"/>
         <m u="1"/>
       </sharedItems>
+    </cacheField>
+    <cacheField name="Is passive" numFmtId="0">
+      <sharedItems containsBlank="1"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -2043,6 +1927,7 @@
     <d v="2023-12-27T20:03:00"/>
     <d v="1899-12-30T03:02:00"/>
     <x v="0"/>
+    <m/>
   </r>
   <r>
     <s v="Play Test"/>
@@ -2052,6 +1937,7 @@
     <m/>
     <d v="1899-12-30T00:30:00"/>
     <x v="1"/>
+    <b v="1"/>
   </r>
   <r>
     <s v="TimeManagment maintenance"/>
@@ -2061,15 +1947,17 @@
     <m/>
     <d v="1899-12-30T01:02:00"/>
     <x v="1"/>
+    <b v="1"/>
   </r>
   <r>
     <s v="Make low HP visuals"/>
     <m/>
     <x v="2"/>
     <d v="2023-12-28T08:57:00"/>
-    <m/>
+    <d v="2023-12-28T09:30:00"/>
     <d v="1899-12-30T00:25:00"/>
-    <x v="1"/>
+    <x v="0"/>
+    <m/>
   </r>
   <r>
     <s v="Implement low HP visuals"/>
@@ -2079,6 +1967,7 @@
     <d v="2023-12-28T16:06:00"/>
     <d v="1899-12-30T02:38:00"/>
     <x v="0"/>
+    <m/>
   </r>
   <r>
     <s v="Make falling sprite + polish sprite sheet"/>
@@ -2088,15 +1977,17 @@
     <d v="2023-12-28T11:24:00"/>
     <d v="1899-12-30T01:16:00"/>
     <x v="0"/>
+    <m/>
   </r>
   <r>
     <s v="Implement new sprite sheet (polish)"/>
     <m/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <s v="Not started"/>
-    <x v="1"/>
+    <d v="2024-01-01T20:00:00"/>
+    <d v="2024-01-01T22:41:00"/>
+    <d v="1899-12-30T02:09:00"/>
+    <x v="0"/>
+    <m/>
   </r>
   <r>
     <s v="Improve global structure"/>
@@ -2104,8 +1995,9 @@
     <x v="3"/>
     <d v="2023-12-28T16:06:00"/>
     <m/>
-    <d v="1899-12-30T00:47:00"/>
+    <d v="1899-12-30T00:53:00"/>
     <x v="1"/>
+    <b v="1"/>
   </r>
   <r>
     <s v="Correct small bugs"/>
@@ -2115,382 +2007,424 @@
     <m/>
     <s v="Not started"/>
     <x v="1"/>
+    <b v="1"/>
   </r>
   <r>
-    <m/>
+    <s v="Create new levels (level design)"/>
     <m/>
     <x v="4"/>
+    <m/>
+    <m/>
+    <s v="Not started"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
+    <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
     <m/>
     <s v=""/>
     <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="6">
+      <items count="7">
         <item x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item x="5"/>
         <item x="4"/>
         <item t="default"/>
       </items>
@@ -2499,19 +2433,22 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+      <items count="7">
+        <item m="1" x="4"/>
+        <item m="1" x="3"/>
+        <item h="1" m="1" x="5"/>
+        <item h="1" x="2"/>
+        <item x="0"/>
         <item x="1"/>
-        <item x="0"/>
-        <item h="1" m="1" x="3"/>
-        <item h="1" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -2523,6 +2460,9 @@
     </i>
     <i>
       <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
@@ -2538,7 +2478,7 @@
     <dataField name="Somme de Total time" fld="5" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="30">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2566,39 +2506,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:H50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="11">
       <calculatedColumnFormula>_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="9">
       <calculatedColumnFormula>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:E50" xr:uid="{341A430F-6539-4177-979B-C2093504802E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="12">
       <calculatedColumnFormula>IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2872,8 +2812,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,15 +2889,12 @@
 )</f>
         <v>0.12638888888614019</v>
       </c>
-      <c r="G2" s="23" t="str">
+      <c r="G2" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="K2" s="2"/>
       <c r="L2" s="8" t="b">
         <f>1=1</f>
@@ -2986,7 +2923,7 @@
 )</f>
         <v>2.0833333335758653E-2</v>
       </c>
-      <c r="G3" s="23" t="str">
+      <c r="G3" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>NO</v>
       </c>
@@ -2994,8 +2931,8 @@
         <v>1</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="9" t="s">
-        <v>16</v>
+      <c r="J3" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="10" t="b">
@@ -3025,7 +2962,7 @@
 )</f>
         <v>4.3055555550381541E-2</v>
       </c>
-      <c r="G4" s="23" t="str">
+      <c r="G4" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>NO</v>
       </c>
@@ -3034,7 +2971,7 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="9" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -3061,14 +2998,14 @@
 )</f>
         <v>1.7361111116770189E-2</v>
       </c>
-      <c r="G5" s="23" t="str">
+      <c r="G5" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -3095,14 +3032,14 @@
 )</f>
         <v>0.10972222221607808</v>
       </c>
-      <c r="G6" s="23" t="str">
+      <c r="G6" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="9" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -3129,14 +3066,14 @@
 )</f>
         <v>5.2777777775190771E-2</v>
       </c>
-      <c r="G7" s="23" t="str">
+      <c r="G7" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="11" t="s">
-        <v>12</v>
+      <c r="J7" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -3149,23 +3086,29 @@
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="D8" s="13">
+        <v>45292.833333333336</v>
+      </c>
+      <c r="E8" s="13">
+        <v>45292.945138888892</v>
+      </c>
+      <c r="F8" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
-      </c>
-      <c r="G8" s="23" t="str">
+        <v>8.9583333334303461E-2</v>
+      </c>
+      <c r="G8" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
@@ -3189,13 +3132,17 @@
 )</f>
         <v>3.680555555911269E-2</v>
       </c>
-      <c r="G9" s="23" t="str">
+      <c r="G9" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>NO</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
@@ -3217,33 +3164,41 @@
 )</f>
         <v>Not started</v>
       </c>
-      <c r="G10" s="23" t="str">
+      <c r="G10" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>NO</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="13"/>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="13">
+        <v>45293.916666666664</v>
+      </c>
       <c r="E11" s="13"/>
-      <c r="F11" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="F11" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
-      </c>
-      <c r="G11" s="23" t="str">
+        <v>8.9583333334303461E-2</v>
+      </c>
+      <c r="G11" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -3252,10 +3207,16 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="13"/>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="13">
+        <v>45293.038888888892</v>
+      </c>
       <c r="E12" s="13"/>
       <c r="F12" s="4" t="str">
         <f>_xlfn.LET(
@@ -3263,11 +3224,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
-      </c>
-      <c r="G12" s="23" t="str">
+        <v>Not started</v>
+      </c>
+      <c r="G12" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -3289,7 +3250,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G13" s="23" t="str">
+      <c r="G13" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3313,7 +3274,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G14" s="23" t="str">
+      <c r="G14" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3337,7 +3298,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G15" s="23" t="str">
+      <c r="G15" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3361,7 +3322,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G16" s="23" t="str">
+      <c r="G16" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3385,7 +3346,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G17" s="23" t="str">
+      <c r="G17" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3409,7 +3370,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G18" s="23" t="str">
+      <c r="G18" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3433,7 +3394,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G19" s="23" t="str">
+      <c r="G19" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3457,7 +3418,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G20" s="23" t="str">
+      <c r="G20" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3481,7 +3442,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G21" s="23" t="str">
+      <c r="G21" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3505,7 +3466,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G22" s="23" t="str">
+      <c r="G22" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3529,7 +3490,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G23" s="23" t="str">
+      <c r="G23" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3553,7 +3514,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G24" s="23" t="str">
+      <c r="G24" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3577,7 +3538,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G25" s="23" t="str">
+      <c r="G25" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3601,7 +3562,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G26" s="23" t="str">
+      <c r="G26" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3625,7 +3586,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G27" s="23" t="str">
+      <c r="G27" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3649,7 +3610,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G28" s="23" t="str">
+      <c r="G28" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3673,7 +3634,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G29" s="23" t="str">
+      <c r="G29" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3697,7 +3658,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G30" s="23" t="str">
+      <c r="G30" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3721,7 +3682,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G31" s="23" t="str">
+      <c r="G31" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3745,7 +3706,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G32" s="23" t="str">
+      <c r="G32" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3769,7 +3730,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G33" s="23" t="str">
+      <c r="G33" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3793,7 +3754,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G34" s="23" t="str">
+      <c r="G34" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3817,7 +3778,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G35" s="23" t="str">
+      <c r="G35" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3841,7 +3802,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G36" s="23" t="str">
+      <c r="G36" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3865,7 +3826,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G37" s="23" t="str">
+      <c r="G37" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3889,7 +3850,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G38" s="23" t="str">
+      <c r="G38" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3913,7 +3874,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G39" s="23" t="str">
+      <c r="G39" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3937,7 +3898,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G40" s="23" t="str">
+      <c r="G40" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3961,7 +3922,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G41" s="23" t="str">
+      <c r="G41" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3985,7 +3946,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G42" s="23" t="str">
+      <c r="G42" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4009,7 +3970,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G43" s="23" t="str">
+      <c r="G43" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4033,7 +3994,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G44" s="23" t="str">
+      <c r="G44" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4057,7 +4018,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G45" s="23" t="str">
+      <c r="G45" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4081,7 +4042,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G46" s="23" t="str">
+      <c r="G46" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4105,7 +4066,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G47" s="23" t="str">
+      <c r="G47" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4129,7 +4090,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G48" s="23" t="str">
+      <c r="G48" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4153,7 +4114,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G49" s="23" t="str">
+      <c r="G49" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4177,7 +4138,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G50" s="23" t="str">
+      <c r="G50" s="24" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4688,31 +4649,31 @@
       <c r="H108" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2:G50">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>$H2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="5">
+      <formula>AND(NOT($G2 = "YES"), $A2 &lt;&gt; "")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>$G2="YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G60:H108">
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>AND(NOT($G60), $A60 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$G60</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G50">
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>$G2="YES"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
-      <formula>AND(NOT($G2 = "YES"), $A2 &lt;&gt; "")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>$H2</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50 C60:C108" xr:uid="{DC5BF156-2602-425B-86A0-7257C6F2DA5F}">
-      <formula1>$J$2:$J$7</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H50" xr:uid="{D6219296-ED51-4D3C-BCB2-1138D9D7567E}">
       <formula1>$L$2:$L$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50 C60:C108" xr:uid="{DC5BF156-2602-425B-86A0-7257C6F2DA5F}">
+      <formula1>$J$3:$J$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4727,8 +4688,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4855,13 +4816,13 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.7361111109494232E-2</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -4878,11 +4839,11 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>2.569444444088731E-2</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -4899,14 +4860,14 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>3.5416666665696539E-2</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="21">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>0.40694444443943212</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
+        <v>0.58611111110803904</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -4923,11 +4884,11 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.1111111110949423E-2</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -4996,34 +4957,50 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="17" t="str">
+      <c r="C15" s="12">
+        <v>45292.854166666664</v>
+      </c>
+      <c r="D15" s="12">
+        <v>45292.943749999999</v>
+      </c>
+      <c r="E15" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
-        <v/>
-      </c>
-      <c r="G15" s="24"/>
+        <v>8.9583333334303461E-2</v>
+      </c>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="17" t="str">
+      <c r="C16" s="12">
+        <v>45292.949305555558</v>
+      </c>
+      <c r="D16" s="12">
+        <v>45293.038888888892</v>
+      </c>
+      <c r="E16" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
-        <v/>
+        <v>8.9583333334303461E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="12"/>
+      <c r="C17" s="12">
+        <v>45293.039583333331</v>
+      </c>
       <c r="D17" s="12"/>
       <c r="E17" s="17" t="str">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
-        <v/>
+        <v>(Current session) 0h 00m</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -5385,7 +5362,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5421,7 +5398,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="16">
-        <v>0.1423611111111111</v>
+        <v>0.23611111111111113</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5450,10 +5427,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="16">
-        <v>0.40277777777777779</v>
+      <c r="B9" s="16">
+        <v>0.49652777777777779</v>
       </c>
     </row>
     <row r="28" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
polished level 1 and 2
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51933E3A-3DDB-4528-8FCF-1590BCEC2C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DD8A0C-2069-4927-9662-6DA50622A087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>Correct tilemap collider</t>
+  </si>
+  <si>
+    <t>Implement milk low hp (blend tree)</t>
+  </si>
+  <si>
+    <t>Make collectibles assets</t>
+  </si>
+  <si>
+    <t>Implement collectibles</t>
+  </si>
+  <si>
+    <t>Update camera visuals to take into account camera size</t>
   </si>
 </sst>
 </file>
@@ -369,6 +381,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -384,26 +399,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <fill>
         <patternFill>
@@ -445,49 +445,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="2" tint="-0.499984740745262"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
     </dxf>
     <dxf>
@@ -598,6 +555,52 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
     </dxf>
     <dxf>
       <font>
@@ -1036,19 +1039,19 @@
                 <c:formatCode>h"h"\ mm"min";@</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.23611111111111113</c:v>
+                  <c:v>0.46319444444444452</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.16944444444444445</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>3.6111111111111115E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.013888888888889E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>8.9583333333333334E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1865,7 +1868,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45292.949456365743" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45293.964090046298" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tasks"/>
   </cacheSource>
@@ -1887,10 +1890,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Started" numFmtId="167">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2024-01-01T20:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2024-01-02T22:00:00"/>
     </cacheField>
     <cacheField name="Ended" numFmtId="167">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2024-01-01T22:41:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2024-01-02T01:57:00"/>
     </cacheField>
     <cacheField name="Total time" numFmtId="165">
       <sharedItems containsDate="1" containsMixedTypes="1" minDate="1899-12-30T00:25:00" maxDate="1899-12-30T03:02:00"/>
@@ -1935,7 +1938,7 @@
     <x v="1"/>
     <d v="2023-12-27T16:45:00"/>
     <m/>
-    <d v="1899-12-30T00:30:00"/>
+    <d v="1899-12-30T00:52:00"/>
     <x v="1"/>
     <b v="1"/>
   </r>
@@ -2005,7 +2008,7 @@
     <x v="3"/>
     <m/>
     <m/>
-    <s v="Not started"/>
+    <d v="1899-12-30T02:14:00"/>
     <x v="1"/>
     <b v="1"/>
   </r>
@@ -2013,30 +2016,30 @@
     <s v="Create new levels (level design)"/>
     <m/>
     <x v="4"/>
-    <m/>
-    <m/>
-    <s v="Not started"/>
+    <d v="2024-01-02T22:00:00"/>
+    <m/>
+    <d v="1899-12-30T02:09:00"/>
     <x v="1"/>
     <m/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
-    <m/>
+    <s v="Correct tilemap collider"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-02T00:56:00"/>
+    <d v="2024-01-02T01:57:00"/>
+    <d v="1899-12-30T00:59:00"/>
+    <x v="0"/>
+    <b v="0"/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
+    <s v="Implement milk low hp (blend tree)"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-02T01:56:00"/>
+    <m/>
+    <d v="1899-12-30T02:14:00"/>
+    <x v="1"/>
     <m/>
   </r>
   <r>
@@ -2413,7 +2416,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -2478,7 +2481,7 @@
     <dataField name="Somme de Total time" fld="5" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="3">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2506,39 +2509,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:H50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="15">
       <calculatedColumnFormula>_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="9">
+    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="14">
       <calculatedColumnFormula>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:E50" xr:uid="{341A430F-6539-4177-979B-C2093504802E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="6">
       <calculatedColumnFormula>IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2813,12 +2816,12 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
     <col min="2" max="2" width="74.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
@@ -2889,7 +2892,7 @@
 )</f>
         <v>0.12638888888614019</v>
       </c>
-      <c r="G2" s="24" t="str">
+      <c r="G2" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
@@ -2921,9 +2924,9 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>2.0833333335758653E-2</v>
-      </c>
-      <c r="G3" s="24" t="str">
+        <v>3.6111111112404615E-2</v>
+      </c>
+      <c r="G3" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>NO</v>
       </c>
@@ -2962,7 +2965,7 @@
 )</f>
         <v>4.3055555550381541E-2</v>
       </c>
-      <c r="G4" s="24" t="str">
+      <c r="G4" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>NO</v>
       </c>
@@ -2998,7 +3001,7 @@
 )</f>
         <v>1.7361111116770189E-2</v>
       </c>
-      <c r="G5" s="24" t="str">
+      <c r="G5" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
@@ -3032,7 +3035,7 @@
 )</f>
         <v>0.10972222221607808</v>
       </c>
-      <c r="G6" s="24" t="str">
+      <c r="G6" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
@@ -3066,7 +3069,7 @@
 )</f>
         <v>5.2777777775190771E-2</v>
       </c>
-      <c r="G7" s="24" t="str">
+      <c r="G7" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
@@ -3100,7 +3103,7 @@
 )</f>
         <v>8.9583333334303461E-2</v>
       </c>
-      <c r="G8" s="24" t="str">
+      <c r="G8" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
@@ -3132,7 +3135,7 @@
 )</f>
         <v>3.680555555911269E-2</v>
       </c>
-      <c r="G9" s="24" t="str">
+      <c r="G9" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>NO</v>
       </c>
@@ -3156,15 +3159,15 @@
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="F10" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
-      </c>
-      <c r="G10" s="24" t="str">
+        <v>9.3055555553291924E-2</v>
+      </c>
+      <c r="G10" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>NO</v>
       </c>
@@ -3194,9 +3197,9 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>8.9583333334303461E-2</v>
-      </c>
-      <c r="G11" s="24" t="str">
+        <v>0.13333333333866904</v>
+      </c>
+      <c r="G11" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>NO</v>
       </c>
@@ -3217,42 +3220,52 @@
       <c r="D12" s="13">
         <v>45293.038888888892</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="E12" s="13">
+        <v>45293.081250000003</v>
+      </c>
+      <c r="F12" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
-      </c>
-      <c r="G12" s="24" t="str">
+        <v>4.0972222224809229E-2</v>
+      </c>
+      <c r="G12" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v>NO</v>
-      </c>
-      <c r="H12" s="2"/>
+        <v>YES</v>
+      </c>
+      <c r="H12" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="13"/>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="13">
+        <v>45293.080555555556</v>
+      </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="F13" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
-      </c>
-      <c r="G13" s="24" t="str">
+        <v>9.3055555553291924E-2</v>
+      </c>
+      <c r="G13" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -3261,9 +3274,13 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="4" t="str">
@@ -3272,11 +3289,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
-      </c>
-      <c r="G14" s="24" t="str">
+        <v>Not started</v>
+      </c>
+      <c r="G14" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -3285,9 +3302,13 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="4" t="str">
@@ -3296,11 +3317,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
-      </c>
-      <c r="G15" s="24" t="str">
+        <v>Not started</v>
+      </c>
+      <c r="G15" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -3309,10 +3330,16 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="13">
+        <v>45294.648611111108</v>
+      </c>
       <c r="E16" s="13"/>
       <c r="F16" s="4" t="str">
         <f>_xlfn.LET(
@@ -3320,11 +3347,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
-      </c>
-      <c r="G16" s="24" t="str">
+        <v>Not started</v>
+      </c>
+      <c r="G16" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3346,7 +3373,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G17" s="24" t="str">
+      <c r="G17" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3370,7 +3397,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G18" s="24" t="str">
+      <c r="G18" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3394,7 +3421,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G19" s="24" t="str">
+      <c r="G19" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3418,7 +3445,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G20" s="24" t="str">
+      <c r="G20" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3442,7 +3469,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G21" s="24" t="str">
+      <c r="G21" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3466,7 +3493,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G22" s="24" t="str">
+      <c r="G22" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3490,7 +3517,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G23" s="24" t="str">
+      <c r="G23" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3514,7 +3541,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G24" s="24" t="str">
+      <c r="G24" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3538,7 +3565,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G25" s="24" t="str">
+      <c r="G25" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3562,7 +3589,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G26" s="24" t="str">
+      <c r="G26" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3586,7 +3613,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G27" s="24" t="str">
+      <c r="G27" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3610,7 +3637,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G28" s="24" t="str">
+      <c r="G28" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3634,7 +3661,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G29" s="24" t="str">
+      <c r="G29" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3658,7 +3685,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G30" s="24" t="str">
+      <c r="G30" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3682,7 +3709,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G31" s="24" t="str">
+      <c r="G31" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3706,7 +3733,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G32" s="24" t="str">
+      <c r="G32" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3730,7 +3757,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G33" s="24" t="str">
+      <c r="G33" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3754,7 +3781,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G34" s="24" t="str">
+      <c r="G34" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3778,7 +3805,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G35" s="24" t="str">
+      <c r="G35" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3802,7 +3829,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G36" s="24" t="str">
+      <c r="G36" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3826,7 +3853,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G37" s="24" t="str">
+      <c r="G37" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3850,7 +3877,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G38" s="24" t="str">
+      <c r="G38" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3874,7 +3901,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G39" s="24" t="str">
+      <c r="G39" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3898,7 +3925,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G40" s="24" t="str">
+      <c r="G40" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3922,7 +3949,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G41" s="24" t="str">
+      <c r="G41" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3946,7 +3973,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G42" s="24" t="str">
+      <c r="G42" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3970,7 +3997,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G43" s="24" t="str">
+      <c r="G43" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -3994,7 +4021,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G44" s="24" t="str">
+      <c r="G44" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4018,7 +4045,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G45" s="24" t="str">
+      <c r="G45" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4042,7 +4069,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G46" s="24" t="str">
+      <c r="G46" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4066,7 +4093,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G47" s="24" t="str">
+      <c r="G47" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4090,7 +4117,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G48" s="24" t="str">
+      <c r="G48" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4114,7 +4141,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G49" s="24" t="str">
+      <c r="G49" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4138,7 +4165,7 @@
 )</f>
         <v/>
       </c>
-      <c r="G50" s="24" t="str">
+      <c r="G50" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v/>
       </c>
@@ -4650,21 +4677,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G50">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$H2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>AND(NOT($G2 = "YES"), $A2 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$G2="YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:H108">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>AND(NOT($G60), $A60 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$G60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4689,15 +4716,15 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="1" max="1" width="56.42578125" customWidth="1"/>
     <col min="2" max="2" width="86.5703125" customWidth="1"/>
-    <col min="3" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="43.28515625" customWidth="1"/>
+    <col min="3" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -4816,13 +4843,13 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.7361111109494232E-2</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -4839,11 +4866,11 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>2.569444444088731E-2</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -4860,14 +4887,14 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>3.5416666665696539E-2</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="22">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>0.58611111110803904</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
+        <v>0.87222222222044365</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -4884,11 +4911,11 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
         <v>1.1111111110949423E-2</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -4997,60 +5024,88 @@
       <c r="C17" s="12">
         <v>45293.039583333331</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="17" t="str">
+      <c r="D17" s="12">
+        <v>45293.080555555556</v>
+      </c>
+      <c r="E17" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
-        <v>(Current session) 0h 00m</v>
+        <v>4.0972222224809229E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="17" t="str">
+      <c r="C18" s="12">
+        <v>45293.081250000003</v>
+      </c>
+      <c r="D18" s="12">
+        <v>45293.174305555556</v>
+      </c>
+      <c r="E18" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
-        <v/>
+        <v>9.3055555553291924E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="17" t="str">
+      <c r="C19" s="12">
+        <v>45293.174305555556</v>
+      </c>
+      <c r="D19" s="12">
+        <v>45293.267361111109</v>
+      </c>
+      <c r="E19" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
-        <v/>
+        <v>9.3055555553291924E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="17" t="str">
+      <c r="C20" s="12">
+        <v>45293.828472222223</v>
+      </c>
+      <c r="D20" s="12">
+        <v>45293.84375</v>
+      </c>
+      <c r="E20" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
-        <v/>
+        <v>1.5277777776645962E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="17" t="str">
+      <c r="C21" s="12">
+        <v>45294.604166666664</v>
+      </c>
+      <c r="D21" s="12">
+        <v>45294.647916666669</v>
+      </c>
+      <c r="E21" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
-        <v/>
+        <v>4.3750000004365575E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B22" s="2"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="17" t="str">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)"" h""h"" mm""m""")), "")</f>
-        <v/>
+        <v>(Current session) 15h 34m</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -5359,10 +5414,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F34BC3-EAE3-4982-A7A6-05997E0322BF}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5375,9 +5430,10 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -5385,7 +5441,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>31</v>
       </c>
@@ -5393,15 +5449,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="16">
-        <v>0.23611111111111113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.46319444444444452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
@@ -5409,37 +5465,64 @@
         <v>0.16944444444444445</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="16">
-        <v>2.0833333333333332E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.6111111111111115E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="16">
         <v>7.013888888888889E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="K7" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8.9583333333333334E-2</v>
+      </c>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="16">
-        <v>0.49652777777777779</v>
-      </c>
+        <v>0.82847222222222228</v>
+      </c>
+      <c r="K9" s="22">
+        <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
+        <v>0.87222222222044365</v>
+      </c>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
     </row>
     <row r="28" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
@@ -5447,6 +5530,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K7:O8"/>
+    <mergeCell ref="K9:O10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
revised level 3 and refractored levels
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,20 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBDB44F-5B86-448C-96E0-9597329D8CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3181012-A4A3-415B-92E9-781C778EAACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="Sessions track" sheetId="2" r:id="rId2"/>
     <sheet name="Charts" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Segment_Finished">#N/A</definedName>
+    <definedName name="Segment_Is_passive">#N/A</definedName>
+    <definedName name="Segment_Task_Type">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
+      <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicerCache r:id="rId5"/>
+        <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
+      </x15:slicerCaches>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -41,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -195,6 +210,15 @@
   <si>
     <t>Papa</t>
   </si>
+  <si>
+    <t>Desolidarize the path module from EnemyController</t>
+  </si>
+  <si>
+    <t>Add stun parameter to enemies</t>
+  </si>
+  <si>
+    <t>It should if not null override the hurting frames of the player</t>
+  </si>
 </sst>
 </file>
 
@@ -206,7 +230,7 @@
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
     <numFmt numFmtId="167" formatCode="d/m/yy\ hh:mm;@"/>
     <numFmt numFmtId="168" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
-    <numFmt numFmtId="170" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
+    <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -397,23 +421,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1838,6 +1856,245 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1790700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3619500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Task Type">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A46F1627-7ABB-A234-5804-E61E9B0827A3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Task Type"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1790700" y="4124325"/>
+              <a:ext cx="1828800" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="fr-FR" sz="1100"/>
+                <a:t>Cette forme représente un segment de table. Les segments de table ne sont pas pris en charge dans cette version d’Excel.
+En revanche, si la forme a été modifiée dans une version antérieure d’Excel, ou si le classeur a été enregistré dans Excel 2007 ou une version antérieure, vous ne pouvez pas utiliser le segment.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1847850</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Finished">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAAAC74E-E0C0-4AD3-2676-A8D124B8B746}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Finished"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3848100" y="4124325"/>
+              <a:ext cx="1828800" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="fr-FR" sz="1100"/>
+                <a:t>Cette forme représente un segment de table. Les segments de table ne sont pas pris en charge dans cette version d’Excel.
+En revanche, si la forme a été modifiée dans une version antérieure d’Excel, ou si le classeur a été enregistré dans Excel 2007 ou une version antérieure, vous ne pouvez pas utiliser le segment.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1933575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3762375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Is passive">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1A9A0DA-FDCC-1E1C-F141-41F1EE06C8E3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Is passive"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5762625" y="4124325"/>
+              <a:ext cx="1828800" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="fr-FR" sz="1100"/>
+                <a:t>Cette forme représente un segment de table. Les segments de table ne sont pas pris en charge dans cette version d’Excel.
+En revanche, si la forme a été modifiée dans une version antérieure d’Excel, ou si le classeur a été enregistré dans Excel 2007 ou une version antérieure, vous ne pouvez pas utiliser le segment.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -2426,7 +2683,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -2491,7 +2748,7 @@
     <dataField name="Somme de Total time" fld="5" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="8">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2518,41 +2775,79 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Segment_Task_Type" xr10:uid="{C70863E4-4BCF-4A27-8CDB-CDC3EBC70F84}" sourceName="Task Type">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="1" column="3"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Segment_Finished" xr10:uid="{65C2FCDD-E499-40F9-8707-413F382090EF}" sourceName="Finished">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="1" column="7"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Segment_Is_passive" xr10:uid="{C0D5C3BB-AA55-4AEE-A914-725134A2E58E}" sourceName="Is passive">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="1" column="9"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Task Type" xr10:uid="{ABB9CCB1-71E5-45FC-BB3E-FB77B047FBCB}" cache="Segment_Task_Type" caption="Task Type" rowHeight="241300"/>
+  <slicer name="Finished" xr10:uid="{005FB207-8F62-4702-97C5-70A11EE60090}" cache="Segment_Finished" caption="Finished" rowHeight="241300"/>
+  <slicer name="Is passive" xr10:uid="{89E5B2FD-3CB1-4E79-98C3-BDC34A77EE4A}" cache="Segment_Is_passive" caption="Is passive" rowHeight="241300"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:H50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="15">
       <calculatedColumnFormula>_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="16">
+    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="14">
       <calculatedColumnFormula>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:E50" xr:uid="{341A430F-6539-4177-979B-C2093504802E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="2">
-      <calculatedColumnFormula>IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="0">
+      <calculatedColumnFormula>IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2825,8 +3120,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3167,7 +3462,9 @@
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D10" s="13">
+        <v>45296</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="4">
         <f ca="1">_xlfn.LET(
@@ -3245,9 +3542,7 @@
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
         <v>YES</v>
       </c>
-      <c r="H12" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -3350,7 +3645,9 @@
       <c r="D16" s="13">
         <v>45294.648611111108</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="13">
+        <v>45294.779166666667</v>
+      </c>
       <c r="F16" s="4">
         <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
@@ -3361,7 +3658,7 @@
       </c>
       <c r="G16" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3370,9 +3667,13 @@
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="4" t="str">
@@ -3381,11 +3682,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G17" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3394,9 +3695,15 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="4" t="str">
@@ -3405,11 +3712,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G18" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -4687,21 +4994,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G50">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$H2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>AND(NOT($G2 = "YES"), $A2 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$G2="YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:H108">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND(NOT($G60), $A60 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$G60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4714,9 +5021,17 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
+      <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4726,7 +5041,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4734,7 +5049,7 @@
     <col min="1" max="1" width="56.42578125" customWidth="1"/>
     <col min="2" max="2" width="86.5703125" customWidth="1"/>
     <col min="3" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -4766,7 +5081,7 @@
         <v>45287.834722222222</v>
       </c>
       <c r="E2" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>0.12638888888614019</v>
       </c>
     </row>
@@ -4784,7 +5099,7 @@
         <v>45287.708333333336</v>
       </c>
       <c r="E3" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.0416666671517305E-2</v>
       </c>
     </row>
@@ -4800,7 +5115,7 @@
         <v>45288.361805555556</v>
       </c>
       <c r="E4" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.7361111109494232E-2</v>
       </c>
     </row>
@@ -4818,7 +5133,7 @@
         <v>45288.372916666667</v>
       </c>
       <c r="E5" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.0416666664241347E-2</v>
       </c>
     </row>
@@ -4834,7 +5149,7 @@
         <v>45288.395833333336</v>
       </c>
       <c r="E6" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.7361111116770189E-2</v>
       </c>
     </row>
@@ -4850,7 +5165,7 @@
         <v>45288.413194444445</v>
       </c>
       <c r="E7" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.7361111109494232E-2</v>
       </c>
       <c r="F7" s="20" t="s">
@@ -4873,7 +5188,7 @@
         <v>45288.439583333333</v>
       </c>
       <c r="E8" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>2.569444444088731E-2</v>
       </c>
       <c r="F8" s="21"/>
@@ -4894,7 +5209,7 @@
         <v>45288.474999999999</v>
       </c>
       <c r="E9" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>3.5416666665696539E-2</v>
       </c>
       <c r="F9" s="22">
@@ -4918,7 +5233,7 @@
         <v>45288.488888888889</v>
       </c>
       <c r="E10" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.1111111110949423E-2</v>
       </c>
       <c r="F10" s="23"/>
@@ -4939,7 +5254,7 @@
         <v>45288.540277777778</v>
       </c>
       <c r="E11" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>8.333333331393078E-3</v>
       </c>
     </row>
@@ -4955,7 +5270,7 @@
         <v>45288.67083333333</v>
       </c>
       <c r="E12" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>9.0277777773735579E-2</v>
       </c>
     </row>
@@ -4973,7 +5288,7 @@
         <v>45288.70416666667</v>
       </c>
       <c r="E13" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>3.2638888893416151E-2</v>
       </c>
     </row>
@@ -4989,7 +5304,7 @@
         <v>45288.738194444442</v>
       </c>
       <c r="E14" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>4.166666665696539E-3</v>
       </c>
     </row>
@@ -5005,7 +5320,7 @@
         <v>45292.943749999999</v>
       </c>
       <c r="E15" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>8.9583333334303461E-2</v>
       </c>
       <c r="G15" s="18"/>
@@ -5022,7 +5337,7 @@
         <v>45293.038888888892</v>
       </c>
       <c r="E16" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>8.9583333334303461E-2</v>
       </c>
     </row>
@@ -5038,7 +5353,7 @@
         <v>45293.080555555556</v>
       </c>
       <c r="E17" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>4.0972222224809229E-2</v>
       </c>
     </row>
@@ -5054,7 +5369,7 @@
         <v>45293.174305555556</v>
       </c>
       <c r="E18" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>9.3055555553291924E-2</v>
       </c>
     </row>
@@ -5070,7 +5385,7 @@
         <v>45293.267361111109</v>
       </c>
       <c r="E19" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>9.3055555553291924E-2</v>
       </c>
     </row>
@@ -5088,7 +5403,7 @@
         <v>45293.84375</v>
       </c>
       <c r="E20" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.5277777776645962E-2</v>
       </c>
     </row>
@@ -5104,7 +5419,7 @@
         <v>45294.647916666669</v>
       </c>
       <c r="E21" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>4.3750000004365575E-2</v>
       </c>
     </row>
@@ -5120,7 +5435,7 @@
         <v>45294.779166666667</v>
       </c>
       <c r="E22" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>0.13055555555911269</v>
       </c>
     </row>
@@ -5138,18 +5453,22 @@
         <v>45294.788194444445</v>
       </c>
       <c r="E23" s="17">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.3888888890505768E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="12"/>
+      <c r="C24" s="12">
+        <v>45296.541666666664</v>
+      </c>
       <c r="D24" s="12"/>
       <c r="E24" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
+        <v>(Current session) 3h 52m</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -5158,7 +5477,7 @@
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5168,7 +5487,7 @@
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5178,7 +5497,7 @@
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5188,7 +5507,7 @@
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5198,7 +5517,7 @@
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5208,7 +5527,7 @@
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5218,7 +5537,7 @@
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5228,7 +5547,7 @@
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5238,7 +5557,7 @@
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5248,7 +5567,7 @@
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5258,7 +5577,7 @@
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5268,7 +5587,7 @@
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5278,7 +5597,7 @@
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5288,7 +5607,7 @@
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5298,7 +5617,7 @@
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5308,7 +5627,7 @@
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5318,7 +5637,7 @@
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5328,7 +5647,7 @@
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5338,7 +5657,7 @@
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
       <c r="E43" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5348,7 +5667,7 @@
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5358,7 +5677,7 @@
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="E45" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5368,7 +5687,7 @@
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5378,7 +5697,7 @@
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5388,7 +5707,7 @@
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5398,7 +5717,7 @@
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5408,7 +5727,7 @@
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="17" t="str">
-        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session)""[h]""h"" mm""m""")), "")</f>
+        <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v/>
       </c>
     </row>
@@ -5441,7 +5760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F34BC3-EAE3-4982-A7A6-05997E0322BF}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
set up maxsize camera option
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68082CA9-7AF5-4381-B805-611109FD8A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B986DD6B-6D70-4955-BD2D-1C1B96924FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -225,6 +225,18 @@
   <si>
     <t>levels 3 and partially 4</t>
   </si>
+  <si>
+    <t>Detect player fell</t>
+  </si>
+  <si>
+    <t>Implement falling platform</t>
+  </si>
+  <si>
+    <t>Create assets falling platform</t>
+  </si>
+  <si>
+    <t>advanced lv 4</t>
+  </si>
 </sst>
 </file>
 
@@ -380,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -433,31 +445,14 @@
     <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="24">
     <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
+      <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
     </dxf>
     <dxf>
       <fill>
@@ -501,6 +496,21 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
     </dxf>
     <dxf>
       <font>
@@ -1881,8 +1891,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Task Type">
@@ -1905,7 +1915,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1959,8 +1969,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Finished">
@@ -1983,7 +1993,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2037,8 +2047,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Is passive">
@@ -2061,7 +2071,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2695,7 +2705,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -2759,9 +2769,12 @@
   <dataFields count="1">
     <dataField name="Somme de Total time" fld="5" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="8">
+  <formats count="2">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="0">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <chartFormats count="1">
@@ -2826,39 +2839,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:H50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="16">
       <calculatedColumnFormula>_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="16">
+    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="15">
       <calculatedColumnFormula>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E50" xr:uid="{341A430F-6539-4177-979B-C2093504802E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="7">
       <calculatedColumnFormula>IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3133,7 +3146,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3516,7 +3529,7 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>0.29513888889778173</v>
+        <v>0.34097222223499557</v>
       </c>
       <c r="G11" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
@@ -3737,9 +3750,13 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="4" t="str">
@@ -3748,11 +3765,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G19" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -3761,9 +3778,13 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="4" t="str">
@@ -3772,11 +3793,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G20" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3785,9 +3806,13 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="4" t="str">
@@ -3796,11 +3821,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G21" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -5006,21 +5031,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G50">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$H2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>AND(NOT($G2 = "YES"), $A2 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$G2="YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:H108">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND(NOT($G60), $A60 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$G60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5053,7 +5078,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5226,7 +5251,7 @@
       </c>
       <c r="F9" s="22">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.1784722222291748</v>
+        <v>1.2243055555663886</v>
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
@@ -5490,23 +5515,35 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="17" t="str">
+      <c r="A25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="12">
+        <v>45297.588194444441</v>
+      </c>
+      <c r="D25" s="12">
+        <v>45297.634027777778</v>
+      </c>
+      <c r="E25" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>4.5833333337213844E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="12"/>
+      <c r="C26" s="12">
+        <v>45297.634027777778</v>
+      </c>
       <c r="D26" s="12"/>
       <c r="E26" s="17" t="str">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>(Current session) 0h 00m</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -5779,7 +5816,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5867,12 +5904,12 @@
       <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="24">
         <v>1.0166666666666668</v>
       </c>
       <c r="K9" s="22">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.1784722222291748</v>
+        <v>1.2243055555663886</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>

</xml_diff>

<commit_message>
falling platform + finished lv4
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B986DD6B-6D70-4955-BD2D-1C1B96924FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA54B41B-AE86-4991-AAF0-E74DFF7598B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -1891,8 +1891,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Task Type">
@@ -1915,7 +1915,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3146,7 +3146,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3529,7 +3529,7 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>0.34097222223499557</v>
+        <v>0.41736111112550134</v>
       </c>
       <c r="G11" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
@@ -3785,19 +3785,23 @@
       <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="D20" s="13">
+        <v>45297.644444444442</v>
+      </c>
+      <c r="E20" s="13">
+        <v>45297.75</v>
+      </c>
+      <c r="F20" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
+        <v>0.10694444444379769</v>
       </c>
       <c r="G20" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3813,19 +3817,23 @@
       <c r="C21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="D21" s="13">
+        <v>45297.644444444442</v>
+      </c>
+      <c r="E21" s="13">
+        <v>45297.75</v>
+      </c>
+      <c r="F21" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
+        <v>8.333333331393078E-3</v>
       </c>
       <c r="G21" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -5078,7 +5086,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5251,7 +5259,7 @@
       </c>
       <c r="F9" s="22">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.2243055555663886</v>
+        <v>1.4159722222320852</v>
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
@@ -5540,30 +5548,44 @@
       <c r="C26" s="12">
         <v>45297.634027777778</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="17" t="str">
+      <c r="D26" s="12">
+        <v>45297.642361111109</v>
+      </c>
+      <c r="E26" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v>(Current session) 0h 00m</v>
+        <v>8.333333331393078E-3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="17" t="str">
+      <c r="C27" s="12">
+        <v>45297.643055555556</v>
+      </c>
+      <c r="D27" s="12">
+        <v>45297.75</v>
+      </c>
+      <c r="E27" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>0.10694444444379769</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="17" t="str">
+      <c r="C28" s="12">
+        <v>45297.75</v>
+      </c>
+      <c r="D28" s="12">
+        <v>45297.826388888891</v>
+      </c>
+      <c r="E28" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>7.6388888890505768E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -5909,7 +5931,7 @@
       </c>
       <c r="K9" s="22">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.2243055555663886</v>
+        <v>1.4159722222320852</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>

</xml_diff>

<commit_message>
created struct for damage data
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA54B41B-AE86-4991-AAF0-E74DFF7598B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF76170B-8DB1-4DB4-B4B9-89EE5D291363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Motive (task)</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Session start</t>
   </si>
   <si>
@@ -236,6 +233,18 @@
   </si>
   <si>
     <t>advanced lv 4</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Fix ahead camera</t>
+  </si>
+  <si>
+    <t>Added a phase parameter</t>
+  </si>
+  <si>
+    <t>Struct for damage</t>
   </si>
 </sst>
 </file>
@@ -392,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -433,6 +442,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -445,15 +455,12 @@
     <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
-    <dxf>
-      <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -493,6 +500,9 @@
           <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
@@ -1882,17 +1892,17 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1790700</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3619500</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Task Type">
@@ -1915,7 +1925,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1960,13 +1970,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2038,13 +2048,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1933575</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3762375</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2773,7 +2783,7 @@
     <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="5">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2840,7 +2850,16 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:H50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}"/>
+  <autoFilter ref="A1:H50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="20"/>
@@ -2868,7 +2887,7 @@
   <autoFilter ref="A1:E50" xr:uid="{341A430F-6539-4177-979B-C2093504802E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Description" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Comment" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="7">
@@ -3146,7 +3165,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3187,7 +3206,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="5" t="s">
@@ -3198,7 +3217,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3234,7 +3253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -3273,7 +3292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -3304,12 +3323,12 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -3343,7 +3362,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -3377,7 +3396,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -3411,9 +3430,9 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -3445,9 +3464,9 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -3479,9 +3498,9 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -3513,11 +3532,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="13">
         <v>45293.916666666664</v>
@@ -3541,9 +3560,9 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -3575,7 +3594,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -3605,7 +3624,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -3633,7 +3652,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
@@ -3659,9 +3678,9 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
@@ -3691,27 +3710,31 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="D17" s="13">
+        <v>45297.865972222222</v>
+      </c>
+      <c r="E17" s="13">
+        <v>45297.95416666667</v>
+      </c>
+      <c r="F17" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
+        <v>8.6805555554747116E-2</v>
       </c>
       <c r="G17" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3721,23 +3744,25 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="13">
+        <v>45297.95416666667</v>
+      </c>
       <c r="E18" s="13"/>
-      <c r="F18" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="F18" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
+        <v>1.6666666662786156E-2</v>
       </c>
       <c r="G18" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
@@ -3751,7 +3776,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -3777,9 +3802,9 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -3809,9 +3834,9 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -3842,9 +3867,13 @@
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="4" t="str">
@@ -3853,11 +3882,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G22" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3865,7 +3894,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3889,7 +3918,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3913,7 +3942,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3937,7 +3966,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3961,7 +3990,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3985,7 +4014,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -4009,7 +4038,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4033,7 +4062,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -4057,7 +4086,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4081,7 +4110,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4105,7 +4134,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4129,7 +4158,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -4153,7 +4182,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -4177,7 +4206,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -4201,7 +4230,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -4225,7 +4254,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -4249,7 +4278,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -4273,7 +4302,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -4297,7 +4326,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -4321,7 +4350,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -4345,7 +4374,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -4369,7 +4398,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -4393,7 +4422,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -4417,7 +4446,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -4441,7 +4470,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -4465,7 +4494,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -4489,7 +4518,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -4513,7 +4542,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -5039,21 +5068,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G50">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$H2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>AND(NOT($G2 = "YES"), $A2 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$G2="YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:H108">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>AND(NOT($G60), $A60 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$G60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5085,8 +5114,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5102,16 +5131,16 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5135,7 +5164,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="12">
         <v>45287.697916666664</v>
@@ -5169,7 +5198,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="12">
         <v>45288.362500000003</v>
@@ -5213,13 +5242,13 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.7361111109494232E-2</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
+      <c r="F7" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -5236,11 +5265,11 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>2.569444444088731E-2</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -5257,14 +5286,14 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>3.5416666665696539E-2</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.4159722222320852</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
+        <v>1.5194444444496185</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -5281,11 +5310,11 @@
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
         <v>1.1111111110949423E-2</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -5321,10 +5350,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C13" s="12">
         <v>45288.671527777777</v>
@@ -5339,7 +5368,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="12">
@@ -5355,7 +5384,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="12">
@@ -5372,7 +5401,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="12">
@@ -5388,7 +5417,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="12">
@@ -5404,7 +5433,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="12">
@@ -5420,7 +5449,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="12">
@@ -5439,7 +5468,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="12">
         <v>45293.828472222223</v>
@@ -5454,10 +5483,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="12">
         <v>45294.604166666664</v>
@@ -5472,7 +5501,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="12">
@@ -5491,7 +5520,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="12">
         <v>45294.774305555555</v>
@@ -5506,10 +5535,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="12">
         <v>45296.541666666664</v>
@@ -5524,10 +5553,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="12">
         <v>45297.588194444441</v>
@@ -5542,7 +5571,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="12">
@@ -5558,7 +5587,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="12">
@@ -5574,7 +5603,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="12">
@@ -5589,29 +5618,45 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="17" t="str">
+      <c r="A29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="12">
+        <v>45297.865972222222</v>
+      </c>
+      <c r="D29" s="12">
+        <v>45297.952777777777</v>
+      </c>
+      <c r="E29" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>8.6805555554747116E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="17" t="str">
+      <c r="A30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="12">
+        <v>45297.95416666667</v>
+      </c>
+      <c r="D30" s="12">
+        <v>45297.970833333333</v>
+      </c>
+      <c r="E30" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>1.6666666662786156E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="12"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="12"/>
       <c r="E31" s="17" t="str">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
@@ -5859,15 +5904,15 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -5901,53 +5946,53 @@
       <c r="B7" s="16">
         <v>7.013888888888889E-2</v>
       </c>
-      <c r="K7" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
+      <c r="K7" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="16">
         <v>0.13333333333333333</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="24">
+        <v>31</v>
+      </c>
+      <c r="B9" s="20">
         <v>1.0166666666666668</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.4159722222320852</v>
-      </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
+        <v>1.5194444444496185</v>
+      </c>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
     </row>
     <row r="28" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ko sound and fixed lv 2 + 3
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89D433D-5D6F-445D-A304-47A27F91DC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D189847-2994-4B04-842A-84C906305A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>new damage sound for falling</t>
+  </si>
+  <si>
+    <t>Find KO sound</t>
+  </si>
+  <si>
+    <t>Implement KO sound</t>
   </si>
 </sst>
 </file>
@@ -465,20 +471,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
     </dxf>
     <dxf>
       <fill>
@@ -505,121 +503,6 @@
           <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -714,6 +597,135 @@
     <dxf>
       <font>
         <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1076,9 +1088,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Charts!$A$4:$A$9</c:f>
+              <c:f>Charts!$A$4:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Coding</c:v>
                 </c:pt>
@@ -1094,17 +1106,20 @@
                 <c:pt idx="4">
                   <c:v>Level design</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>Audio assets</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$B$4:$B$9</c:f>
+              <c:f>Charts!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>h"h"\ mm"min";@</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.59375000000000011</c:v>
+                  <c:v>0.91319444444444453</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.16944444444444445</c:v>
@@ -1113,10 +1128,13 @@
                   <c:v>4.9999999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.013888888888889E-2</c:v>
+                  <c:v>7.8472222222222221E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13333333333333333</c:v>
+                  <c:v>0.41736111111111113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1111111111111112E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1897,13 +1915,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1790700</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3619500</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -1975,13 +1993,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2053,13 +2071,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1933575</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3762375</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2172,7 +2190,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45296.70345277778" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45298.980123148147" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tasks"/>
   </cacheSource>
@@ -2184,23 +2202,24 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Task Type" numFmtId="0">
-      <sharedItems containsBlank="1" count="6">
+      <sharedItems containsBlank="1" count="7">
         <s v="Management"/>
         <s v="Playtesting"/>
         <s v="Sprite assets"/>
         <s v="Coding"/>
         <s v="Level design"/>
+        <s v="Audio assets"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Started" numFmtId="167">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2024-01-06T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2024-01-07T23:10:00"/>
     </cacheField>
     <cacheField name="Ended" numFmtId="167">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2024-01-03T18:42:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2024-01-07T23:27:00"/>
     </cacheField>
     <cacheField name="Total time" numFmtId="165">
-      <sharedItems containsDate="1" containsMixedTypes="1" minDate="1899-12-30T00:25:00" maxDate="1899-12-30T03:12:00"/>
+      <sharedItems containsDate="1" containsMixedTypes="1" minDate="1899-12-30T00:12:00" maxDate="1899-12-30T10:01:00"/>
     </cacheField>
     <cacheField name="Finished" numFmtId="0">
       <sharedItems containsBlank="1" count="6">
@@ -2322,7 +2341,7 @@
     <x v="4"/>
     <d v="2024-01-02T22:00:00"/>
     <m/>
-    <d v="1899-12-30T03:12:00"/>
+    <d v="1899-12-30T10:01:00"/>
     <x v="1"/>
     <m/>
   </r>
@@ -2380,26 +2399,86 @@
     <s v="Desolidarize the path module from EnemyController"/>
     <m/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <s v="Not started"/>
-    <x v="1"/>
+    <d v="2024-01-06T20:47:00"/>
+    <d v="2024-01-06T22:54:00"/>
+    <d v="1899-12-30T02:05:00"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="Add stun parameter to enemies"/>
     <s v="It should if not null override the hurting frames of the player"/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <s v="Not started"/>
-    <x v="1"/>
+    <d v="2024-01-06T22:54:00"/>
+    <d v="2024-01-07T19:34:00"/>
+    <d v="1899-12-30T01:18:00"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
-    <m/>
+    <s v="Detect player fell"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-07T20:22:00"/>
+    <d v="2024-01-07T21:06:00"/>
+    <d v="1899-12-30T00:32:00"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Implement falling platform"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-06T15:28:00"/>
+    <d v="2024-01-06T18:00:00"/>
+    <d v="1899-12-30T02:34:00"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Create assets falling platform"/>
+    <m/>
+    <x v="2"/>
+    <d v="2024-01-06T15:28:00"/>
+    <d v="2024-01-06T18:00:00"/>
+    <d v="1899-12-30T00:12:00"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Fix ahead camera"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-07T21:06:00"/>
+    <d v="2024-01-07T22:00:00"/>
+    <d v="1899-12-30T00:54:00"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Find KO sound"/>
     <m/>
     <x v="5"/>
+    <d v="2024-01-07T23:00:00"/>
+    <d v="2024-01-07T23:10:00"/>
+    <d v="1899-12-30T00:16:00"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Implement KO sound"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-07T23:10:00"/>
+    <d v="2024-01-07T23:27:00"/>
+    <d v="1899-12-30T00:17:00"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2409,7 +2488,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2419,7 +2498,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2429,7 +2508,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2439,7 +2518,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2449,7 +2528,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2459,7 +2538,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2469,7 +2548,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2479,7 +2558,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2489,7 +2568,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2499,7 +2578,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2509,7 +2588,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2519,7 +2598,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2529,7 +2608,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2539,7 +2618,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2549,7 +2628,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2559,7 +2638,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2569,7 +2648,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2579,7 +2658,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2589,7 +2668,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2599,7 +2678,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2609,7 +2688,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2619,7 +2698,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2629,7 +2708,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2639,7 +2718,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2649,67 +2728,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="5"/>
+    <x v="6"/>
     <m/>
     <m/>
     <s v=""/>
@@ -2720,19 +2739,20 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="7">
+      <items count="8">
         <item x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item x="6"/>
+        <item x="4"/>
         <item x="5"/>
-        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2755,7 +2775,7 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -2771,6 +2791,9 @@
     <i>
       <x v="5"/>
     </i>
+    <i>
+      <x v="6"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -2785,10 +2808,10 @@
     <dataField name="Somme de Total time" fld="5" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="6">
+    <format dxfId="18">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="17">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2854,48 +2877,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:H50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="NO"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="7">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="15">
+    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="6">
       <calculatedColumnFormula>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:E50" xr:uid="{341A430F-6539-4177-979B-C2093504802E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Comment" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Comment" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="19">
       <calculatedColumnFormula>IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3170,7 +3188,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3222,7 +3240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3333,7 +3351,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -3367,7 +3385,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -3401,7 +3419,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -3435,7 +3453,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -3565,7 +3583,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -3683,7 +3701,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -3715,7 +3733,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -3747,7 +3765,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -3781,7 +3799,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
@@ -3813,7 +3831,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
@@ -3845,7 +3863,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -3888,18 +3906,20 @@
       <c r="D22" s="13">
         <v>45298.879166666666</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="E22" s="13">
+        <v>45298.916666666664</v>
+      </c>
+      <c r="F22" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
+        <v>3.7499999998544808E-2</v>
       </c>
       <c r="G22" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3907,23 +3927,31 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="C23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="13">
+        <v>45298.958333333336</v>
+      </c>
+      <c r="E23" s="13">
+        <v>45298.965277777781</v>
+      </c>
+      <c r="F23" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>1.1111111110949423E-2</v>
       </c>
       <c r="G23" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>YES</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3931,23 +3959,31 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="C24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="13">
+        <v>45298.965277777781</v>
+      </c>
+      <c r="E24" s="13">
+        <v>45298.977083333331</v>
+      </c>
+      <c r="F24" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>1.1805555550381541E-2</v>
       </c>
       <c r="G24" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>YES</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -3955,7 +3991,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3979,7 +4015,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -4003,7 +4039,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -4027,7 +4063,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -4051,7 +4087,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4075,7 +4111,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -4099,7 +4135,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4123,7 +4159,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4147,7 +4183,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4171,7 +4207,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -4195,7 +4231,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -4219,7 +4255,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -4243,7 +4279,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -4267,7 +4303,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -4291,7 +4327,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -4315,7 +4351,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -4339,7 +4375,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -4363,7 +4399,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -4387,7 +4423,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -4411,7 +4447,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -4435,7 +4471,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -4459,7 +4495,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -4483,7 +4519,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -4507,7 +4543,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -4531,7 +4567,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -4555,7 +4591,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -5092,10 +5128,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:H108">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>AND(NOT($G60), $A60 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>$G60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5128,7 +5164,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5301,7 +5337,7 @@
       </c>
       <c r="F9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.5791666666700621</v>
+        <v>1.6395833333299379</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -5710,30 +5746,44 @@
       <c r="C33" s="12">
         <v>45298.879166666666</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="17" t="str">
+      <c r="D33" s="12">
+        <v>45298.916666666664</v>
+      </c>
+      <c r="E33" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v>(Current session) 0h 00m</v>
+        <v>3.7499999998544808E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="17" t="str">
+      <c r="C34" s="12">
+        <v>45298.95416666667</v>
+      </c>
+      <c r="D34" s="12">
+        <v>45298.965277777781</v>
+      </c>
+      <c r="E34" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>1.1111111110949423E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="17" t="str">
+      <c r="C35" s="12">
+        <v>45298.965277777781</v>
+      </c>
+      <c r="D35" s="12">
+        <v>45298.977083333331</v>
+      </c>
+      <c r="E35" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>1.1805555550381541E-2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -5916,7 +5966,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5953,7 +6003,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="16">
-        <v>0.59375000000000011</v>
+        <v>0.91319444444444453</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -5977,7 +6027,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="16">
-        <v>7.013888888888889E-2</v>
+        <v>7.8472222222222221E-2</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>39</v>
@@ -5992,7 +6042,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="16">
-        <v>0.13333333333333333</v>
+        <v>0.41736111111111113</v>
       </c>
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
@@ -6002,14 +6052,14 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="20">
-        <v>1.0166666666666668</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="16">
+        <v>1.1111111111111112E-2</v>
       </c>
       <c r="K9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.5791666666700621</v>
+        <v>1.6395833333299379</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
@@ -6017,6 +6067,12 @@
       <c r="O9" s="23"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="20">
+        <v>1.6395833333333334</v>
+      </c>
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>

</xml_diff>

<commit_message>
refractored and advanced to lv5
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D189847-2994-4B04-842A-84C906305A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4DB22A-2F26-4EF3-9255-0DB5E8776438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -471,12 +471,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="24">
     <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -503,6 +511,121 @@
           <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Avenir Next LT Pro"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -597,135 +720,6 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="[h]&quot;h&quot;\ mm&quot;m&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="h&quot;h&quot;\ mm&quot;min&quot;;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="h&quot;h&quot;\ mm&quot;m&quot;;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Avenir Next LT Pro"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2739,7 +2733,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DD6E2B2-CA8C-4658-80FD-EC26C6D715A5}" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -2808,10 +2802,10 @@
     <dataField name="Somme de Total time" fld="5" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="18">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="5">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2877,43 +2871,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}" name="Tasks" displayName="Tasks" ref="A1:H50" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:H50" xr:uid="{FEAE4602-F0F4-4371-84F1-3AFAD46F0CA7}">
     <filterColumn colId="7">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{8B27624E-49A7-450F-BE7E-731DE5DB093F}" name="Feature/Task" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C36AF95D-C9FF-4855-BBA9-5546049AA39F}" name="Desciption" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{CBBD0622-A516-452B-B94A-8291C5109D06}" name="Task Type" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{1619EB2C-9622-44DA-83E6-5D0AFCA0617E}" name="Started" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{5DA25ECD-2C10-4535-9FE4-35E696C5C386}" name="Ended" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{721FF157-37F6-46FB-9684-6BDD8317DA66}" name="Total time" dataDxfId="16">
       <calculatedColumnFormula>_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{790641DF-098B-4245-A927-B76CD5EBC543}" name="Finished" dataDxfId="15">
       <calculatedColumnFormula>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{58D2A8C5-189A-420E-B31D-1D70DDBB9854}" name="Is passive" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E50" xr:uid="{341A430F-6539-4177-979B-C2093504802E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Comment" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Comment" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{6DC14596-976B-4CBE-B8C2-123BDF384988}" name="Session start" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{67A0A396-2632-44ED-B680-1E5AB83AE86D}" name="Session end" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{4EEF71A5-3355-4270-A56F-4B00DAC175A2}" name="Session time" dataDxfId="7">
       <calculatedColumnFormula>IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3188,7 +3182,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5128,10 +5122,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:H108">
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>AND(NOT($G60), $A60 &lt;&gt; "")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$G60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5164,7 +5158,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5787,13 +5781,17 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="12"/>
+      <c r="C36" s="12">
+        <v>45304.695833333331</v>
+      </c>
       <c r="D36" s="12"/>
       <c r="E36" s="17" t="str">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>(Current session) 0h 00m</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
heart gun complete !
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4DB22A-2F26-4EF3-9255-0DB5E8776438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4DCA7C-C9D1-45B2-8DB5-EBFFFD677E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>Implement KO sound</t>
+  </si>
+  <si>
+    <t>Implement heart projectiles</t>
   </si>
 </sst>
 </file>
@@ -2902,6 +2905,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{341A430F-6539-4177-979B-C2093504802E}" name="Sessions" displayName="Sessions" ref="A1:E50" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E50" xr:uid="{341A430F-6539-4177-979B-C2093504802E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E50">
+    <sortCondition ref="C1:C50"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{64088F67-E263-4A55-9EAF-D34F094ED468}" name="Motive (task)" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{C78510A6-72A3-4D34-A5CB-7F3FF3553696}" name="Comment" dataDxfId="10"/>
@@ -3182,7 +3188,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3565,7 +3571,7 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>0.41736111112550134</v>
+        <v>0.4638888889021473</v>
       </c>
       <c r="G11" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
@@ -3986,10 +3992,16 @@
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="13"/>
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="13">
+        <v>45304.743055555555</v>
+      </c>
       <c r="E25" s="13"/>
       <c r="F25" s="4" t="str">
         <f>_xlfn.LET(
@@ -3997,11 +4009,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G25" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -5157,8 +5169,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5188,36 +5200,36 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C2" s="12">
+        <v>45287.697916666664</v>
+      </c>
+      <c r="D2" s="12">
         <v>45287.708333333336</v>
-      </c>
-      <c r="D2" s="12">
-        <v>45287.834722222222</v>
       </c>
       <c r="E2" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v>0.12638888888614019</v>
+        <v>1.0416666671517305E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="12">
-        <v>45287.697916666664</v>
+        <v>45287.708333333336</v>
       </c>
       <c r="D3" s="12">
-        <v>45287.708333333336</v>
+        <v>45287.834722222222</v>
       </c>
       <c r="E3" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v>1.0416666671517305E-2</v>
+        <v>0.12638888888614019</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -5331,7 +5343,7 @@
       </c>
       <c r="F9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.6395833333299379</v>
+        <v>1.6861111111065838</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -5788,20 +5800,26 @@
       <c r="C36" s="12">
         <v>45304.695833333331</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="17" t="str">
+      <c r="D36" s="12">
+        <v>45304.742361111108</v>
+      </c>
+      <c r="E36" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v>(Current session) 0h 00m</v>
+        <v>4.6527777776645962E-2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
+      <c r="A37" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="12"/>
+      <c r="C37" s="12">
+        <v>45304.743055555555</v>
+      </c>
       <c r="D37" s="12"/>
       <c r="E37" s="17" t="str">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>(Current session) 0h 00m</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -6057,7 +6075,7 @@
       </c>
       <c r="K9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>1.6395833333299379</v>
+        <v>1.6861111111065838</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>

</xml_diff>

<commit_message>
-------- now using forces for milk !
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B94A4C-E576-40F9-84AF-FA596CCEF26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC684A2-BC1E-4BD4-8F16-D01C5C05236A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>Create destructable walls</t>
+  </si>
+  <si>
+    <t>Warn player for their new power</t>
+  </si>
+  <si>
+    <t>Fix platform and use forces instead of velocity</t>
   </si>
 </sst>
 </file>
@@ -1936,13 +1942,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1790700</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3619500</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2014,13 +2020,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2092,13 +2098,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1933575</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3762375</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -3217,7 +3223,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3600,7 +3606,7 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>0.4638888889021473</v>
+        <v>0.54652777779119788</v>
       </c>
       <c r="G11" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
@@ -4178,7 +4184,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>73</v>
       </c>
@@ -4211,7 +4217,9 @@
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
         <v>18</v>
@@ -4224,11 +4232,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G31" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -4237,10 +4245,16 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+      <c r="A32" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="13"/>
+      <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="13">
+        <v>45306</v>
+      </c>
       <c r="E32" s="13"/>
       <c r="F32" s="4" t="str">
         <f>_xlfn.LET(
@@ -4248,11 +4262,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G32" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -5240,8 +5254,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5414,7 +5428,7 @@
       </c>
       <c r="F9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>2.0722222222320852</v>
+        <v>2.1548611111211358</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -5999,20 +6013,26 @@
       <c r="C44" s="12">
         <v>45305.917361111111</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="17" t="str">
+      <c r="D44" s="12">
+        <v>45306</v>
+      </c>
+      <c r="E44" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v>(Current session) 0h 11m</v>
+        <v>8.2638888889050577E-2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="12"/>
+      <c r="C45" s="12">
+        <v>45306</v>
+      </c>
       <c r="D45" s="12"/>
       <c r="E45" s="17" t="str">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>(Current session) 2h 48m</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -6188,7 +6208,7 @@
       </c>
       <c r="K9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>2.0722222222320852</v>
+        <v>2.1548611111211358</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>

</xml_diff>

<commit_message>
fixed sprite sheet physics
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC684A2-BC1E-4BD4-8F16-D01C5C05236A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55B6CBF-0358-4361-A042-045237608966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="77">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>Fix platform and use forces instead of velocity</t>
+  </si>
+  <si>
+    <t>useless. forces are cool but impossible to climb ramps + doesn't fix the platform</t>
   </si>
 </sst>
 </file>
@@ -4256,13 +4259,13 @@
         <v>45306</v>
       </c>
       <c r="E32" s="13"/>
-      <c r="F32" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="F32" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
+        <v>0.17708333333575865</v>
       </c>
       <c r="G32" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
@@ -5254,8 +5257,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5428,7 +5431,7 @@
       </c>
       <c r="F9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>2.1548611111211358</v>
+        <v>2.3319444444568944</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -6025,14 +6028,18 @@
       <c r="A45" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="C45" s="12">
         <v>45306</v>
       </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="17" t="str">
+      <c r="D45" s="12">
+        <v>45306.177083333336</v>
+      </c>
+      <c r="E45" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v>(Current session) 2h 48m</v>
+        <v>0.17708333333575865</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -6208,7 +6215,7 @@
       </c>
       <c r="K9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>2.1548611111211358</v>
+        <v>2.3319444444568944</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>

</xml_diff>

<commit_message>
refracted and corrected some bugs
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55B6CBF-0358-4361-A042-045237608966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2069B84D-4B0C-40AD-A35B-8E79FE4BC17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="79">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t>useless. forces are cool but impossible to climb ramps + doesn't fix the platform</t>
+  </si>
+  <si>
+    <t>Revert back to velocity</t>
+  </si>
+  <si>
+    <t>Power ups visual</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1155,7 @@
                 <c:formatCode>h"h"\ mm"min";@</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.10625</c:v>
+                  <c:v>1.2972222222222221</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.16944444444444445</c:v>
@@ -1161,7 +1167,7 @@
                   <c:v>0.23541666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46388888888888885</c:v>
+                  <c:v>0.54652777777777783</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.7222222222222221E-2</c:v>
@@ -1945,13 +1951,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1790700</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3619500</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2023,13 +2029,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2101,13 +2107,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1933575</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3762375</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2220,7 +2226,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45305.917805902776" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45306.937906250001" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tasks"/>
   </cacheSource>
@@ -2243,13 +2249,13 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Started" numFmtId="167">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2024-01-14T13:25:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2024-01-16T00:00:00"/>
     </cacheField>
     <cacheField name="Ended" numFmtId="167">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2024-01-14T22:01:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2024-01-15T18:40:00"/>
     </cacheField>
     <cacheField name="Total time" numFmtId="165">
-      <sharedItems containsDate="1" containsMixedTypes="1" minDate="1899-12-30T00:12:00" maxDate="1899-12-30T11:08:00"/>
+      <sharedItems containsDate="1" containsMixedTypes="1" minDate="1899-12-30T00:12:00" maxDate="1899-12-30T13:07:00"/>
     </cacheField>
     <cacheField name="Finished" numFmtId="0">
       <sharedItems containsBlank="1" count="6">
@@ -2371,7 +2377,7 @@
     <x v="4"/>
     <d v="2024-01-02T22:00:00"/>
     <m/>
-    <d v="1899-12-30T11:08:00"/>
+    <d v="1899-12-30T13:07:00"/>
     <x v="1"/>
     <b v="1"/>
   </r>
@@ -2566,33 +2572,33 @@
     <m/>
   </r>
   <r>
-    <m/>
+    <s v="Warn player for their new power"/>
     <m/>
     <x v="3"/>
     <m/>
     <m/>
-    <s v=""/>
-    <x v="2"/>
+    <s v="Not started"/>
+    <x v="1"/>
     <m/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
+    <s v="Fix platform and use forces instead of velocity"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-15T00:00:00"/>
+    <d v="2024-01-15T18:40:00"/>
+    <d v="1899-12-30T04:15:00"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
+    <s v="Revert back to velocity"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-15T18:20:00"/>
+    <d v="2024-01-15T18:40:00"/>
+    <d v="1899-12-30T00:20:00"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -3226,7 +3232,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3577,7 +3583,7 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>0.14305555555620231</v>
+        <v>0.18472222222044365</v>
       </c>
       <c r="G10" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
@@ -4247,7 +4253,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>75</v>
       </c>
@@ -4258,7 +4264,9 @@
       <c r="D32" s="13">
         <v>45306</v>
       </c>
-      <c r="E32" s="13"/>
+      <c r="E32" s="13">
+        <v>45306.777777777781</v>
+      </c>
       <c r="F32" s="4">
         <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
@@ -4269,7 +4277,7 @@
       </c>
       <c r="G32" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -4277,23 +4285,31 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="C33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="13">
+        <v>45306.763888888891</v>
+      </c>
+      <c r="E33" s="13">
+        <v>45306.777777777781</v>
+      </c>
+      <c r="F33" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>1.3888888890505768E-2</v>
       </c>
       <c r="G33" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>YES</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -4302,10 +4318,16 @@
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="13"/>
+      <c r="C34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="13">
+        <v>45306.979166666664</v>
+      </c>
       <c r="E34" s="13"/>
       <c r="F34" s="4" t="str">
         <f>_xlfn.LET(
@@ -4313,11 +4335,11 @@
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v/>
+        <v>Not started</v>
       </c>
       <c r="G34" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -5257,8 +5279,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5431,7 +5453,7 @@
       </c>
       <c r="F9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>2.3319444444568944</v>
+        <v>2.3875000000116415</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -6043,33 +6065,49 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
+      <c r="A46" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="B46" s="2"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="17" t="str">
+      <c r="C46" s="12">
+        <v>45306.763888888891</v>
+      </c>
+      <c r="D46" s="12">
+        <v>45306.777777777781</v>
+      </c>
+      <c r="E46" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>1.3888888890505768E-2</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
+      <c r="A47" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B47" s="2"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="17" t="str">
+      <c r="C47" s="12">
+        <v>45306.9375</v>
+      </c>
+      <c r="D47" s="12">
+        <v>45306.979166666664</v>
+      </c>
+      <c r="E47" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>4.1666666664241347E-2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
+      <c r="A48" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="B48" s="2"/>
-      <c r="C48" s="12"/>
+      <c r="C48" s="12">
+        <v>45306.979166666664</v>
+      </c>
       <c r="D48" s="12"/>
       <c r="E48" s="17" t="str">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>(Current session) 0h 00m</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -6122,7 +6160,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6159,7 +6197,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="16">
-        <v>1.10625</v>
+        <v>1.2972222222222221</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -6198,7 +6236,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="16">
-        <v>0.46388888888888885</v>
+        <v>0.54652777777777783</v>
       </c>
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
@@ -6215,7 +6253,7 @@
       </c>
       <c r="K9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>2.3319444444568944</v>
+        <v>2.3875000000116415</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
@@ -6227,7 +6265,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="20">
-        <v>2.072222222222222</v>
+        <v>2.3458333333333332</v>
       </c>
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>

</xml_diff>

<commit_message>
particle systems for powerups
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2069B84D-4B0C-40AD-A35B-8E79FE4BC17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD17B354-F7DC-459F-8777-828A89F8F2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="79">
   <si>
     <t>Feature/Task</t>
   </si>
@@ -1951,13 +1951,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1790700</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3619500</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2029,13 +2029,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2107,13 +2107,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1933575</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3762375</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -4233,7 +4233,9 @@
       <c r="C31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="13"/>
+      <c r="D31" s="13">
+        <v>45307.036111111112</v>
+      </c>
       <c r="E31" s="13"/>
       <c r="F31" s="4" t="str">
         <f>_xlfn.LET(
@@ -4317,7 +4319,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
@@ -4328,18 +4330,20 @@
       <c r="D34" s="13">
         <v>45306.979166666664</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="4" t="str">
-        <f>_xlfn.LET(
+      <c r="E34" s="13">
+        <v>45307.036111111112</v>
+      </c>
+      <c r="F34" s="4">
+        <f ca="1">_xlfn.LET(
 _xlpm.totalTime, SUMIFS(Sessions[Session time],Sessions[Session end],"&lt;&gt;",Sessions[Motive (task)],Tasks[[#This Row],[Feature/Task]]),
 _xlpm.taskExists, IF(Tasks[[#This Row],[Feature/Task]] &lt;&gt; "", TRUE, FALSE),
 IF(_xlpm.taskExists,IF(_xlpm.totalTime&lt;&gt;0,_xlpm.totalTime,"Not started"),"")
 )</f>
-        <v>Not started</v>
+        <v>5.6944444448163267E-2</v>
       </c>
       <c r="G34" s="19" t="str">
         <f>IF(Tasks[[#This Row],[Feature/Task]]&lt;&gt;"",IF(Tasks[[#This Row],[Ended]]&lt;&gt; "", "YES", "NO"),"")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -5280,7 +5284,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5453,7 +5457,7 @@
       </c>
       <c r="F9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>2.3875000000116415</v>
+        <v>2.4444444444598048</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -6104,20 +6108,26 @@
       <c r="C48" s="12">
         <v>45306.979166666664</v>
       </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="17" t="str">
+      <c r="D48" s="12">
+        <v>45307.036111111112</v>
+      </c>
+      <c r="E48" s="17">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v>(Current session) 0h 00m</v>
+        <v>5.6944444448163267E-2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="12"/>
+      <c r="C49" s="12">
+        <v>45307.036111111112</v>
+      </c>
       <c r="D49" s="12"/>
       <c r="E49" s="17" t="str">
         <f ca="1">IF(Sessions[[#This Row],[Motive (task)]] &lt;&gt; "", IF(NOT(ISBLANK(Sessions[[#This Row],[Session end]])),Sessions[[#This Row],[Session end]]-Sessions[[#This Row],[Session start]],TEXT(NOW()-Sessions[[#This Row],[Session start]],"""(Current session) ""[h]""h"" mm""m""")), "")</f>
-        <v/>
+        <v>(Current session) 0h 00m</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -6253,7 +6263,7 @@
       </c>
       <c r="K9" s="23">
         <f ca="1" xml:space="preserve"> SUM(Sessions[Session time])</f>
-        <v>2.3875000000116415</v>
+        <v>2.4444444444598048</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>

</xml_diff>

<commit_message>
finished git add .
</commit_message>
<xml_diff>
--- a/Time_Management.xlsx
+++ b/Time_Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AdriKat\Desktop\Projects\Unity\Project - Find Mocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702227A2-0DA8-4D07-9900-AC3B65C3A1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96A1B12-76EA-4F72-9DAC-A28D2C2C8C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -1158,7 +1158,7 @@
                 <c:formatCode>h"h"\ mm"min";@</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.2972222222222221</c:v>
+                  <c:v>1.4402777777777775</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.16944444444444445</c:v>
@@ -2229,7 +2229,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45306.937906250001" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adrien SCHROEDEL" refreshedDate="45312.014070486111" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{C9CE1A9A-A157-4A90-BDFE-1AA8C443533E}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tasks"/>
   </cacheSource>
@@ -2252,10 +2252,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Started" numFmtId="167">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2024-01-16T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T15:25:00" maxDate="2024-01-16T00:52:00"/>
     </cacheField>
     <cacheField name="Ended" numFmtId="167">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2024-01-15T18:40:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-27T20:03:00" maxDate="2024-01-16T00:52:00"/>
     </cacheField>
     <cacheField name="Total time" numFmtId="165">
       <sharedItems containsDate="1" containsMixedTypes="1" minDate="1899-12-30T00:12:00" maxDate="1899-12-30T13:07:00"/>
@@ -2370,7 +2370,7 @@
     <x v="3"/>
     <d v="2024-01-05T00:00:00"/>
     <m/>
-    <d v="1899-12-30T03:26:00"/>
+    <d v="1899-12-30T04:26:00"/>
     <x v="1"/>
     <b v="1"/>
   </r>
@@ -2578,9 +2578,9 @@
     <s v="Warn player for their new power"/>
     <m/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <s v="Not started"/>
+    <d v="2024-01-16T00:52:00"/>
+    <m/>
+    <d v="1899-12-30T00:38:00"/>
     <x v="1"/>
     <m/>
   </r>
@@ -2605,23 +2605,23 @@
     <m/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
+    <s v="Power ups visual"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-15T23:30:00"/>
+    <d v="2024-01-16T00:52:00"/>
+    <d v="1899-12-30T01:22:00"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="2"/>
+    <s v="Add more particles effects"/>
+    <m/>
+    <x v="3"/>
+    <d v="2024-01-16T00:30:00"/>
+    <m/>
+    <d v="1899-12-30T00:26:00"/>
+    <x v="1"/>
     <m/>
   </r>
   <r>
@@ -3234,8 +3234,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5292,8 +5292,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6186,8 +6186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F34BC3-EAE3-4982-A7A6-05997E0322BF}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6224,7 +6224,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="16">
-        <v>1.2972222222222221</v>
+        <v>1.4402777777777775</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -6292,7 +6292,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="20">
-        <v>2.3458333333333332</v>
+        <v>2.4888888888888885</v>
       </c>
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>

</xml_diff>